<commit_message>
Update RPN.xlsx with latest values
</commit_message>
<xml_diff>
--- a/ProcessedData/RPN.xlsx
+++ b/ProcessedData/RPN.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lakshya\Project\ICSS_VSCode\PROJECT\ProcessedData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KOEL\ICSS\Deployment\icss-backend\ProcessedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD40280-1F6A-4E67-9946-3B504338A09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7845"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="321">
   <si>
     <t>Severity (S)</t>
   </si>
@@ -603,12 +604,396 @@
   </si>
   <si>
     <t>Exhaust Manifold</t>
+  </si>
+  <si>
+    <t>LLOP</t>
+  </si>
+  <si>
+    <t>Earth Control Valve</t>
+  </si>
+  <si>
+    <t>Fuse Failure</t>
+  </si>
+  <si>
+    <t>Oil Leakage</t>
+  </si>
+  <si>
+    <t>Oil Drain</t>
+  </si>
+  <si>
+    <t>Exhaust Conical Filter</t>
+  </si>
+  <si>
+    <t>Panel Wiring</t>
+  </si>
+  <si>
+    <t>Silencer</t>
+  </si>
+  <si>
+    <t>Emergency Switch</t>
+  </si>
+  <si>
+    <t>Emergency Stop Button</t>
+  </si>
+  <si>
+    <t>V-Belt</t>
+  </si>
+  <si>
+    <t>Sump</t>
+  </si>
+  <si>
+    <t>Carburettor</t>
+  </si>
+  <si>
+    <t>Exhaust Silencer Flange</t>
+  </si>
+  <si>
+    <t>Hose Clip</t>
+  </si>
+  <si>
+    <t>VMR</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>Mains</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Adblue</t>
+  </si>
+  <si>
+    <t>Alarm</t>
+  </si>
+  <si>
+    <t>Washer</t>
+  </si>
+  <si>
+    <t>Airlock</t>
+  </si>
+  <si>
+    <t>Bellow</t>
+  </si>
+  <si>
+    <t>Rocker Cover</t>
+  </si>
+  <si>
+    <t>T6 Sensor</t>
+  </si>
+  <si>
+    <t>Lube Oil Pressure</t>
+  </si>
+  <si>
+    <t>Exhaust Gas Recirculation</t>
+  </si>
+  <si>
+    <t>Super Capacitor</t>
+  </si>
+  <si>
+    <t>Self-Starter</t>
+  </si>
+  <si>
+    <t>Breather</t>
+  </si>
+  <si>
+    <t>clamp</t>
+  </si>
+  <si>
+    <t>Dipstick</t>
+  </si>
+  <si>
+    <t>Inverter Module</t>
+  </si>
+  <si>
+    <t>Solenoid</t>
+  </si>
+  <si>
+    <t>Engine Hunting</t>
+  </si>
+  <si>
+    <t>Gasket</t>
+  </si>
+  <si>
+    <t>Synchronisation</t>
+  </si>
+  <si>
+    <t>Engine Crank</t>
+  </si>
+  <si>
+    <t>Diesel Leakage</t>
+  </si>
+  <si>
+    <t>AVR</t>
+  </si>
+  <si>
+    <t>Oil Sensor</t>
+  </si>
+  <si>
+    <t>Voltage fluctutation</t>
+  </si>
+  <si>
+    <t>Low Voltage</t>
+  </si>
+  <si>
+    <t>silencer Glading</t>
+  </si>
+  <si>
+    <t>Lug</t>
+  </si>
+  <si>
+    <t>Control Selector</t>
+  </si>
+  <si>
+    <t>Sweep Stuck Alarm</t>
+  </si>
+  <si>
+    <t>CT Neutral</t>
+  </si>
+  <si>
+    <t>Gauge</t>
+  </si>
+  <si>
+    <t>AMF</t>
+  </si>
+  <si>
+    <t>Gas Pressure</t>
+  </si>
+  <si>
+    <t>chock</t>
+  </si>
+  <si>
+    <t>Crank Case</t>
+  </si>
+  <si>
+    <t>Gear Casing</t>
+  </si>
+  <si>
+    <t>Union Thread</t>
+  </si>
+  <si>
+    <t>Adapter</t>
+  </si>
+  <si>
+    <t>MPU</t>
+  </si>
+  <si>
+    <t>Seepage</t>
+  </si>
+  <si>
+    <t>CAC hose</t>
+  </si>
+  <si>
+    <t>Ferule</t>
+  </si>
+  <si>
+    <t>Abnormal</t>
+  </si>
+  <si>
+    <t>DOC</t>
+  </si>
+  <si>
+    <t>Flashing</t>
+  </si>
+  <si>
+    <t>Reverse Power Alarm</t>
+  </si>
+  <si>
+    <t>Banjo</t>
+  </si>
+  <si>
+    <t>Feed Pump</t>
+  </si>
+  <si>
+    <t>Belt Tensioner Meter</t>
+  </si>
+  <si>
+    <t>Ignition Switch</t>
+  </si>
+  <si>
+    <t>Crank Speed Sensor</t>
+  </si>
+  <si>
+    <t>Selector Switch</t>
+  </si>
+  <si>
+    <t>Armature</t>
+  </si>
+  <si>
+    <t>Piston</t>
+  </si>
+  <si>
+    <t>FIP</t>
+  </si>
+  <si>
+    <t>Idle Gear</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Urea Dosing</t>
+  </si>
+  <si>
+    <t>Lube Oil Leakage</t>
+  </si>
+  <si>
+    <t>Allen Key</t>
+  </si>
+  <si>
+    <t>Contactor</t>
+  </si>
+  <si>
+    <t>Turbo Charger</t>
+  </si>
+  <si>
+    <t>Canopy</t>
+  </si>
+  <si>
+    <t>Temperature Switch</t>
+  </si>
+  <si>
+    <t>Control panel</t>
+  </si>
+  <si>
+    <t>Line rejection</t>
+  </si>
+  <si>
+    <t>Fan Pulley</t>
+  </si>
+  <si>
+    <t>Gas filter</t>
+  </si>
+  <si>
+    <t>Bolt</t>
+  </si>
+  <si>
+    <t>ITV</t>
+  </si>
+  <si>
+    <t>Eye Bolt</t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>Fuel Rack</t>
+  </si>
+  <si>
+    <t>Nozzle</t>
+  </si>
+  <si>
+    <t>Valve Bridge</t>
+  </si>
+  <si>
+    <t>MCCB</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>PRV</t>
+  </si>
+  <si>
+    <t>Electric Feed Pump</t>
+  </si>
+  <si>
+    <t>Regulator</t>
+  </si>
+  <si>
+    <t>Exhaust Pipe</t>
+  </si>
+  <si>
+    <t>CT Transformer</t>
+  </si>
+  <si>
+    <t>Engine Block</t>
+  </si>
+  <si>
+    <t>LED Flickering</t>
+  </si>
+  <si>
+    <t>CNC Machine</t>
+  </si>
+  <si>
+    <t>LVM</t>
+  </si>
+  <si>
+    <t>DCU</t>
+  </si>
+  <si>
+    <t>Auto Sensing Cable</t>
+  </si>
+  <si>
+    <t>CAC Pipe</t>
+  </si>
+  <si>
+    <t>Amber Lamp</t>
+  </si>
+  <si>
+    <t>Muffler</t>
+  </si>
+  <si>
+    <t>Stuck Float</t>
+  </si>
+  <si>
+    <t>Fuel float valve</t>
+  </si>
+  <si>
+    <t>Common Rail</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>DPF Weight Measurement</t>
+  </si>
+  <si>
+    <t>Rotor</t>
+  </si>
+  <si>
+    <t>Flash Protect Lamp</t>
+  </si>
+  <si>
+    <t>Governor Spring Pad</t>
+  </si>
+  <si>
+    <t>EMS Switch</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>o-ring</t>
+  </si>
+  <si>
+    <t>Fan Belt</t>
+  </si>
+  <si>
+    <t>Fuel Filter</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Tappet</t>
+  </si>
+  <si>
+    <t>Spark Arrestor</t>
+  </si>
+  <si>
+    <t>Regeneration</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -646,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -657,6 +1042,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,23 +1322,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F186"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F318"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="A320" sqref="A320"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -972,7 +1358,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -992,7 +1378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +1398,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1052,7 +1438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1072,7 +1458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1092,7 +1478,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1112,7 +1498,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1132,7 +1518,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1152,7 +1538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1172,7 +1558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1192,7 +1578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1212,7 +1598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1232,7 +1618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1252,7 +1638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1272,7 +1658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1292,7 +1678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1312,7 +1698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1332,7 +1718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1352,7 +1738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1372,7 +1758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1392,7 +1778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1412,7 +1798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1432,7 +1818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1452,7 +1838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -1472,7 +1858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1492,7 +1878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -1512,7 +1898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -1532,7 +1918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -1552,7 +1938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1572,7 +1958,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1592,7 +1978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1612,7 +1998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>80</v>
       </c>
@@ -1632,7 +2018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>81</v>
       </c>
@@ -1652,7 +2038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>82</v>
       </c>
@@ -1672,7 +2058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>83</v>
       </c>
@@ -1692,7 +2078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>84</v>
       </c>
@@ -1712,7 +2098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>85</v>
       </c>
@@ -1732,7 +2118,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
@@ -1752,7 +2138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
@@ -1772,7 +2158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
@@ -1792,7 +2178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>86</v>
       </c>
@@ -1812,7 +2198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>87</v>
       </c>
@@ -1832,7 +2218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -1852,7 +2238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>89</v>
       </c>
@@ -1872,7 +2258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>90</v>
       </c>
@@ -1892,7 +2278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>91</v>
       </c>
@@ -1912,7 +2298,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>92</v>
       </c>
@@ -1932,7 +2318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>93</v>
       </c>
@@ -1952,7 +2338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>94</v>
       </c>
@@ -1972,7 +2358,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
@@ -1992,7 +2378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -2012,7 +2398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>97</v>
       </c>
@@ -2032,7 +2418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>98</v>
       </c>
@@ -2052,7 +2438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>99</v>
       </c>
@@ -2072,7 +2458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>100</v>
       </c>
@@ -2092,7 +2478,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>101</v>
       </c>
@@ -2112,7 +2498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>40</v>
       </c>
@@ -2132,7 +2518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>41</v>
       </c>
@@ -2152,7 +2538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>102</v>
       </c>
@@ -2172,7 +2558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>103</v>
       </c>
@@ -2192,7 +2578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
@@ -2212,7 +2598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>105</v>
       </c>
@@ -2232,7 +2618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>106</v>
       </c>
@@ -2252,7 +2638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>107</v>
       </c>
@@ -2272,7 +2658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>43</v>
       </c>
@@ -2292,7 +2678,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>44</v>
       </c>
@@ -2312,7 +2698,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>45</v>
       </c>
@@ -2332,7 +2718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>108</v>
       </c>
@@ -2352,7 +2738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>46</v>
       </c>
@@ -2372,7 +2758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>47</v>
       </c>
@@ -2392,7 +2778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>48</v>
       </c>
@@ -2412,7 +2798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>49</v>
       </c>
@@ -2432,7 +2818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>50</v>
       </c>
@@ -2452,7 +2838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -2472,7 +2858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>109</v>
       </c>
@@ -2492,7 +2878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>54</v>
       </c>
@@ -2512,7 +2898,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>52</v>
       </c>
@@ -2532,7 +2918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>110</v>
       </c>
@@ -2552,7 +2938,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>53</v>
       </c>
@@ -2572,7 +2958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>55</v>
       </c>
@@ -2592,7 +2978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>111</v>
       </c>
@@ -2612,7 +2998,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>112</v>
       </c>
@@ -2632,7 +3018,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>113</v>
       </c>
@@ -2652,7 +3038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>114</v>
       </c>
@@ -2672,7 +3058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>115</v>
       </c>
@@ -2692,7 +3078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>116</v>
       </c>
@@ -2712,7 +3098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>117</v>
       </c>
@@ -2732,7 +3118,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>56</v>
       </c>
@@ -2752,7 +3138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>57</v>
       </c>
@@ -2772,7 +3158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>58</v>
       </c>
@@ -2792,7 +3178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>118</v>
       </c>
@@ -2812,7 +3198,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>59</v>
       </c>
@@ -2832,7 +3218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>60</v>
       </c>
@@ -2852,7 +3238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>61</v>
       </c>
@@ -2872,7 +3258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>62</v>
       </c>
@@ -2892,7 +3278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>119</v>
       </c>
@@ -2912,7 +3298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>120</v>
       </c>
@@ -2932,7 +3318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>121</v>
       </c>
@@ -2952,7 +3338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>122</v>
       </c>
@@ -2972,7 +3358,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>123</v>
       </c>
@@ -2992,7 +3378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>124</v>
       </c>
@@ -3012,7 +3398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>125</v>
       </c>
@@ -3032,7 +3418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>126</v>
       </c>
@@ -3052,7 +3438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>127</v>
       </c>
@@ -3072,7 +3458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>128</v>
       </c>
@@ -3092,7 +3478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>129</v>
       </c>
@@ -3112,7 +3498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>130</v>
       </c>
@@ -3132,7 +3518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>131</v>
       </c>
@@ -3152,7 +3538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>132</v>
       </c>
@@ -3172,7 +3558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>133</v>
       </c>
@@ -3192,7 +3578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>134</v>
       </c>
@@ -3212,7 +3598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>135</v>
       </c>
@@ -3232,7 +3618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>136</v>
       </c>
@@ -3252,7 +3638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>137</v>
       </c>
@@ -3272,7 +3658,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>138</v>
       </c>
@@ -3292,7 +3678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>139</v>
       </c>
@@ -3312,7 +3698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>140</v>
       </c>
@@ -3332,7 +3718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>141</v>
       </c>
@@ -3352,7 +3738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>142</v>
       </c>
@@ -3372,7 +3758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>143</v>
       </c>
@@ -3392,7 +3778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>63</v>
       </c>
@@ -3412,7 +3798,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>65</v>
       </c>
@@ -3432,7 +3818,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>66</v>
       </c>
@@ -3452,7 +3838,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>67</v>
       </c>
@@ -3472,7 +3858,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>68</v>
       </c>
@@ -3492,7 +3878,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>69</v>
       </c>
@@ -3512,7 +3898,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>70</v>
       </c>
@@ -3532,7 +3918,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>71</v>
       </c>
@@ -3552,7 +3938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>72</v>
       </c>
@@ -3572,7 +3958,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>73</v>
       </c>
@@ -3592,7 +3978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>74</v>
       </c>
@@ -3612,7 +3998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>75</v>
       </c>
@@ -3632,7 +4018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>76</v>
       </c>
@@ -3652,7 +4038,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>144</v>
       </c>
@@ -3672,7 +4058,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>145</v>
       </c>
@@ -3692,7 +4078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>146</v>
       </c>
@@ -3712,7 +4098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>147</v>
       </c>
@@ -3732,7 +4118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>148</v>
       </c>
@@ -3752,7 +4138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>149</v>
       </c>
@@ -3772,7 +4158,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>150</v>
       </c>
@@ -3792,7 +4178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>151</v>
       </c>
@@ -3812,7 +4198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>152</v>
       </c>
@@ -3832,7 +4218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>153</v>
       </c>
@@ -3852,7 +4238,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>154</v>
       </c>
@@ -3872,7 +4258,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>155</v>
       </c>
@@ -3892,7 +4278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>156</v>
       </c>
@@ -3912,7 +4298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>157</v>
       </c>
@@ -3932,7 +4318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>158</v>
       </c>
@@ -3952,7 +4338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>159</v>
       </c>
@@ -3972,7 +4358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>160</v>
       </c>
@@ -3992,7 +4378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>42</v>
       </c>
@@ -4012,7 +4398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>161</v>
       </c>
@@ -4032,7 +4418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>120</v>
       </c>
@@ -4052,7 +4438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>162</v>
       </c>
@@ -4072,7 +4458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>163</v>
       </c>
@@ -4092,7 +4478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>126</v>
       </c>
@@ -4112,7 +4498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>164</v>
       </c>
@@ -4132,7 +4518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>166</v>
       </c>
@@ -4152,7 +4538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>167</v>
       </c>
@@ -4172,7 +4558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>168</v>
       </c>
@@ -4192,7 +4578,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>169</v>
       </c>
@@ -4212,7 +4598,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>171</v>
       </c>
@@ -4232,7 +4618,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>172</v>
       </c>
@@ -4252,7 +4638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>173</v>
       </c>
@@ -4272,7 +4658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>174</v>
       </c>
@@ -4292,7 +4678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>165</v>
       </c>
@@ -4312,7 +4698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>175</v>
       </c>
@@ -4332,7 +4718,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>176</v>
       </c>
@@ -4352,7 +4738,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>177</v>
       </c>
@@ -4372,7 +4758,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>178</v>
       </c>
@@ -4392,7 +4778,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>179</v>
       </c>
@@ -4412,7 +4798,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>180</v>
       </c>
@@ -4432,7 +4818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>181</v>
       </c>
@@ -4452,7 +4838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>182</v>
       </c>
@@ -4472,7 +4858,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>183</v>
       </c>
@@ -4492,7 +4878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>184</v>
       </c>
@@ -4512,7 +4898,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>185</v>
       </c>
@@ -4532,7 +4918,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>186</v>
       </c>
@@ -4552,7 +4938,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>187</v>
       </c>
@@ -4572,7 +4958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>188</v>
       </c>
@@ -4592,7 +4978,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>189</v>
       </c>
@@ -4612,7 +4998,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>190</v>
       </c>
@@ -4632,7 +5018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>191</v>
       </c>
@@ -4652,7 +5038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>192</v>
       </c>
@@ -4670,6 +5056,2646 @@
       </c>
       <c r="F186" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>193</v>
+      </c>
+      <c r="B187">
+        <v>1</v>
+      </c>
+      <c r="C187">
+        <v>4</v>
+      </c>
+      <c r="D187">
+        <v>10</v>
+      </c>
+      <c r="E187">
+        <v>40</v>
+      </c>
+      <c r="F187" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>194</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="C188">
+        <v>10</v>
+      </c>
+      <c r="D188">
+        <v>2</v>
+      </c>
+      <c r="E188">
+        <v>20</v>
+      </c>
+      <c r="F188" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>195</v>
+      </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
+      <c r="C189">
+        <v>5</v>
+      </c>
+      <c r="D189">
+        <v>4</v>
+      </c>
+      <c r="E189">
+        <v>20</v>
+      </c>
+      <c r="F189" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>196</v>
+      </c>
+      <c r="B190">
+        <v>2</v>
+      </c>
+      <c r="C190">
+        <v>5</v>
+      </c>
+      <c r="D190">
+        <v>9</v>
+      </c>
+      <c r="E190">
+        <v>90</v>
+      </c>
+      <c r="F190" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>197</v>
+      </c>
+      <c r="B191">
+        <v>4</v>
+      </c>
+      <c r="C191">
+        <v>3</v>
+      </c>
+      <c r="D191">
+        <v>9</v>
+      </c>
+      <c r="E191">
+        <v>108</v>
+      </c>
+      <c r="F191" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>198</v>
+      </c>
+      <c r="B192">
+        <v>3</v>
+      </c>
+      <c r="C192">
+        <v>4</v>
+      </c>
+      <c r="D192">
+        <v>4</v>
+      </c>
+      <c r="E192">
+        <v>48</v>
+      </c>
+      <c r="F192" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>199</v>
+      </c>
+      <c r="B193">
+        <v>10</v>
+      </c>
+      <c r="C193">
+        <v>8</v>
+      </c>
+      <c r="D193">
+        <v>5</v>
+      </c>
+      <c r="E193">
+        <v>400</v>
+      </c>
+      <c r="F193" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>200</v>
+      </c>
+      <c r="B194">
+        <v>3</v>
+      </c>
+      <c r="C194">
+        <v>10</v>
+      </c>
+      <c r="D194">
+        <v>9</v>
+      </c>
+      <c r="E194">
+        <v>270</v>
+      </c>
+      <c r="F194" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>201</v>
+      </c>
+      <c r="B195">
+        <v>6</v>
+      </c>
+      <c r="C195">
+        <v>10</v>
+      </c>
+      <c r="D195">
+        <v>9</v>
+      </c>
+      <c r="E195">
+        <v>540</v>
+      </c>
+      <c r="F195" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>202</v>
+      </c>
+      <c r="B196">
+        <v>8</v>
+      </c>
+      <c r="C196">
+        <v>5</v>
+      </c>
+      <c r="D196">
+        <v>5</v>
+      </c>
+      <c r="E196">
+        <v>200</v>
+      </c>
+      <c r="F196" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>313</v>
+      </c>
+      <c r="B197">
+        <v>10</v>
+      </c>
+      <c r="C197">
+        <v>10</v>
+      </c>
+      <c r="D197">
+        <v>1</v>
+      </c>
+      <c r="E197">
+        <v>100</v>
+      </c>
+      <c r="F197" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>203</v>
+      </c>
+      <c r="B198">
+        <v>10</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+      <c r="D198">
+        <v>3</v>
+      </c>
+      <c r="E198">
+        <v>30</v>
+      </c>
+      <c r="F198" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>204</v>
+      </c>
+      <c r="B199">
+        <v>1</v>
+      </c>
+      <c r="C199">
+        <v>5</v>
+      </c>
+      <c r="D199">
+        <v>2</v>
+      </c>
+      <c r="E199">
+        <v>10</v>
+      </c>
+      <c r="F199" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>205</v>
+      </c>
+      <c r="B200">
+        <v>1</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+      <c r="D200">
+        <v>7</v>
+      </c>
+      <c r="E200">
+        <v>7</v>
+      </c>
+      <c r="F200" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>206</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201">
+        <v>2</v>
+      </c>
+      <c r="D201">
+        <v>7</v>
+      </c>
+      <c r="E201">
+        <v>28</v>
+      </c>
+      <c r="F201" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>207</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+      <c r="C202">
+        <v>6</v>
+      </c>
+      <c r="D202">
+        <v>5</v>
+      </c>
+      <c r="E202">
+        <v>60</v>
+      </c>
+      <c r="F202" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>208</v>
+      </c>
+      <c r="B203">
+        <v>1</v>
+      </c>
+      <c r="C203">
+        <v>5</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+      <c r="E203">
+        <v>5</v>
+      </c>
+      <c r="F203" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>209</v>
+      </c>
+      <c r="B204">
+        <v>1</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+      <c r="D204">
+        <v>7</v>
+      </c>
+      <c r="E204">
+        <v>7</v>
+      </c>
+      <c r="F204" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>210</v>
+      </c>
+      <c r="B205">
+        <v>3</v>
+      </c>
+      <c r="C205">
+        <v>8</v>
+      </c>
+      <c r="D205">
+        <v>2</v>
+      </c>
+      <c r="E205">
+        <v>48</v>
+      </c>
+      <c r="F205" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>211</v>
+      </c>
+      <c r="B206">
+        <v>4</v>
+      </c>
+      <c r="C206">
+        <v>5</v>
+      </c>
+      <c r="D206">
+        <v>1</v>
+      </c>
+      <c r="E206">
+        <v>20</v>
+      </c>
+      <c r="F206" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>212</v>
+      </c>
+      <c r="B207">
+        <v>6</v>
+      </c>
+      <c r="C207">
+        <v>4</v>
+      </c>
+      <c r="D207">
+        <v>6</v>
+      </c>
+      <c r="E207">
+        <v>144</v>
+      </c>
+      <c r="F207" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>213</v>
+      </c>
+      <c r="B208">
+        <v>7</v>
+      </c>
+      <c r="C208">
+        <v>8</v>
+      </c>
+      <c r="D208">
+        <v>6</v>
+      </c>
+      <c r="E208">
+        <v>336</v>
+      </c>
+      <c r="F208" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>214</v>
+      </c>
+      <c r="B209">
+        <v>5</v>
+      </c>
+      <c r="C209">
+        <v>9</v>
+      </c>
+      <c r="D209">
+        <v>5</v>
+      </c>
+      <c r="E209">
+        <v>225</v>
+      </c>
+      <c r="F209" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>215</v>
+      </c>
+      <c r="B210">
+        <v>2</v>
+      </c>
+      <c r="C210">
+        <v>9</v>
+      </c>
+      <c r="D210">
+        <v>5</v>
+      </c>
+      <c r="E210">
+        <v>90</v>
+      </c>
+      <c r="F210" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>216</v>
+      </c>
+      <c r="B211">
+        <v>4</v>
+      </c>
+      <c r="C211">
+        <v>8</v>
+      </c>
+      <c r="D211">
+        <v>5</v>
+      </c>
+      <c r="E211">
+        <v>160</v>
+      </c>
+      <c r="F211" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>217</v>
+      </c>
+      <c r="B212">
+        <v>2</v>
+      </c>
+      <c r="C212">
+        <v>8</v>
+      </c>
+      <c r="D212">
+        <v>8</v>
+      </c>
+      <c r="E212">
+        <v>128</v>
+      </c>
+      <c r="F212" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>218</v>
+      </c>
+      <c r="B213">
+        <v>5</v>
+      </c>
+      <c r="C213">
+        <v>9</v>
+      </c>
+      <c r="D213">
+        <v>4</v>
+      </c>
+      <c r="E213">
+        <v>180</v>
+      </c>
+      <c r="F213" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>219</v>
+      </c>
+      <c r="B214">
+        <v>10</v>
+      </c>
+      <c r="C214">
+        <v>2</v>
+      </c>
+      <c r="D214">
+        <v>2</v>
+      </c>
+      <c r="E214">
+        <v>40</v>
+      </c>
+      <c r="F214" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>220</v>
+      </c>
+      <c r="B215">
+        <v>10</v>
+      </c>
+      <c r="C215">
+        <v>10</v>
+      </c>
+      <c r="D215">
+        <v>3</v>
+      </c>
+      <c r="E215">
+        <v>300</v>
+      </c>
+      <c r="F215" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>221</v>
+      </c>
+      <c r="B216">
+        <v>7</v>
+      </c>
+      <c r="C216">
+        <v>4</v>
+      </c>
+      <c r="D216">
+        <v>6</v>
+      </c>
+      <c r="E216">
+        <v>168</v>
+      </c>
+      <c r="F216" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>222</v>
+      </c>
+      <c r="B217">
+        <v>7</v>
+      </c>
+      <c r="C217">
+        <v>9</v>
+      </c>
+      <c r="D217">
+        <v>1</v>
+      </c>
+      <c r="E217">
+        <v>63</v>
+      </c>
+      <c r="F217" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>223</v>
+      </c>
+      <c r="B218">
+        <v>9</v>
+      </c>
+      <c r="C218">
+        <v>9</v>
+      </c>
+      <c r="D218">
+        <v>4</v>
+      </c>
+      <c r="E218">
+        <v>324</v>
+      </c>
+      <c r="F218" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>224</v>
+      </c>
+      <c r="B219">
+        <v>9</v>
+      </c>
+      <c r="C219">
+        <v>10</v>
+      </c>
+      <c r="D219">
+        <v>9</v>
+      </c>
+      <c r="E219">
+        <v>810</v>
+      </c>
+      <c r="F219" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>225</v>
+      </c>
+      <c r="B220">
+        <v>3</v>
+      </c>
+      <c r="C220">
+        <v>7</v>
+      </c>
+      <c r="D220">
+        <v>9</v>
+      </c>
+      <c r="E220">
+        <v>189</v>
+      </c>
+      <c r="F220" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>226</v>
+      </c>
+      <c r="B221">
+        <v>9</v>
+      </c>
+      <c r="C221">
+        <v>4</v>
+      </c>
+      <c r="D221">
+        <v>3</v>
+      </c>
+      <c r="E221">
+        <v>108</v>
+      </c>
+      <c r="F221" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>227</v>
+      </c>
+      <c r="B222">
+        <v>10</v>
+      </c>
+      <c r="C222">
+        <v>3</v>
+      </c>
+      <c r="D222">
+        <v>8</v>
+      </c>
+      <c r="E222">
+        <v>240</v>
+      </c>
+      <c r="F222" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>228</v>
+      </c>
+      <c r="B223">
+        <v>4</v>
+      </c>
+      <c r="C223">
+        <v>7</v>
+      </c>
+      <c r="D223">
+        <v>2</v>
+      </c>
+      <c r="E223">
+        <v>56</v>
+      </c>
+      <c r="F223" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>229</v>
+      </c>
+      <c r="B224">
+        <v>9</v>
+      </c>
+      <c r="C224">
+        <v>4</v>
+      </c>
+      <c r="D224">
+        <v>1</v>
+      </c>
+      <c r="E224">
+        <v>36</v>
+      </c>
+      <c r="F224" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>230</v>
+      </c>
+      <c r="B225">
+        <v>2</v>
+      </c>
+      <c r="C225">
+        <v>3</v>
+      </c>
+      <c r="D225">
+        <v>2</v>
+      </c>
+      <c r="E225">
+        <v>12</v>
+      </c>
+      <c r="F225" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>231</v>
+      </c>
+      <c r="B226">
+        <v>6</v>
+      </c>
+      <c r="C226">
+        <v>4</v>
+      </c>
+      <c r="D226">
+        <v>6</v>
+      </c>
+      <c r="E226">
+        <v>144</v>
+      </c>
+      <c r="F226" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>232</v>
+      </c>
+      <c r="B227">
+        <v>6</v>
+      </c>
+      <c r="C227">
+        <v>7</v>
+      </c>
+      <c r="D227">
+        <v>4</v>
+      </c>
+      <c r="E227">
+        <v>168</v>
+      </c>
+      <c r="F227" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>233</v>
+      </c>
+      <c r="B228">
+        <v>5</v>
+      </c>
+      <c r="C228">
+        <v>7</v>
+      </c>
+      <c r="D228">
+        <v>2</v>
+      </c>
+      <c r="E228">
+        <v>70</v>
+      </c>
+      <c r="F228" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>234</v>
+      </c>
+      <c r="B229">
+        <v>1</v>
+      </c>
+      <c r="C229">
+        <v>8</v>
+      </c>
+      <c r="D229">
+        <v>5</v>
+      </c>
+      <c r="E229">
+        <v>40</v>
+      </c>
+      <c r="F229" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>235</v>
+      </c>
+      <c r="B230">
+        <v>7</v>
+      </c>
+      <c r="C230">
+        <v>9</v>
+      </c>
+      <c r="D230">
+        <v>6</v>
+      </c>
+      <c r="E230">
+        <v>378</v>
+      </c>
+      <c r="F230" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>236</v>
+      </c>
+      <c r="B231">
+        <v>2</v>
+      </c>
+      <c r="C231">
+        <v>7</v>
+      </c>
+      <c r="D231">
+        <v>6</v>
+      </c>
+      <c r="E231">
+        <v>84</v>
+      </c>
+      <c r="F231" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>237</v>
+      </c>
+      <c r="B232">
+        <v>9</v>
+      </c>
+      <c r="C232">
+        <v>10</v>
+      </c>
+      <c r="D232">
+        <v>3</v>
+      </c>
+      <c r="E232">
+        <v>270</v>
+      </c>
+      <c r="F232" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>238</v>
+      </c>
+      <c r="B233">
+        <v>2</v>
+      </c>
+      <c r="C233">
+        <v>4</v>
+      </c>
+      <c r="D233">
+        <v>2</v>
+      </c>
+      <c r="E233">
+        <v>16</v>
+      </c>
+      <c r="F233" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>239</v>
+      </c>
+      <c r="B234">
+        <v>3</v>
+      </c>
+      <c r="C234">
+        <v>7</v>
+      </c>
+      <c r="D234">
+        <v>2</v>
+      </c>
+      <c r="E234">
+        <v>42</v>
+      </c>
+      <c r="F234" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>240</v>
+      </c>
+      <c r="B235">
+        <v>3</v>
+      </c>
+      <c r="C235">
+        <v>4</v>
+      </c>
+      <c r="D235">
+        <v>7</v>
+      </c>
+      <c r="E235">
+        <v>84</v>
+      </c>
+      <c r="F235" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>241</v>
+      </c>
+      <c r="B236">
+        <v>10</v>
+      </c>
+      <c r="C236">
+        <v>6</v>
+      </c>
+      <c r="D236">
+        <v>3</v>
+      </c>
+      <c r="E236">
+        <v>180</v>
+      </c>
+      <c r="F236" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>242</v>
+      </c>
+      <c r="B237">
+        <v>5</v>
+      </c>
+      <c r="C237">
+        <v>5</v>
+      </c>
+      <c r="D237">
+        <v>4</v>
+      </c>
+      <c r="E237">
+        <v>100</v>
+      </c>
+      <c r="F237" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>243</v>
+      </c>
+      <c r="B238">
+        <v>5</v>
+      </c>
+      <c r="C238">
+        <v>9</v>
+      </c>
+      <c r="D238">
+        <v>10</v>
+      </c>
+      <c r="E238">
+        <v>450</v>
+      </c>
+      <c r="F238" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>244</v>
+      </c>
+      <c r="B239">
+        <v>2</v>
+      </c>
+      <c r="C239">
+        <v>9</v>
+      </c>
+      <c r="D239">
+        <v>5</v>
+      </c>
+      <c r="E239">
+        <v>90</v>
+      </c>
+      <c r="F239" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>245</v>
+      </c>
+      <c r="B240">
+        <v>5</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240">
+        <v>3</v>
+      </c>
+      <c r="E240">
+        <v>15</v>
+      </c>
+      <c r="F240" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>246</v>
+      </c>
+      <c r="B241">
+        <v>5</v>
+      </c>
+      <c r="C241">
+        <v>8</v>
+      </c>
+      <c r="D241">
+        <v>1</v>
+      </c>
+      <c r="E241">
+        <v>40</v>
+      </c>
+      <c r="F241" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>247</v>
+      </c>
+      <c r="B242">
+        <v>4</v>
+      </c>
+      <c r="C242">
+        <v>4</v>
+      </c>
+      <c r="D242">
+        <v>5</v>
+      </c>
+      <c r="E242">
+        <v>80</v>
+      </c>
+      <c r="F242" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>248</v>
+      </c>
+      <c r="B243">
+        <v>6</v>
+      </c>
+      <c r="C243">
+        <v>6</v>
+      </c>
+      <c r="D243">
+        <v>5</v>
+      </c>
+      <c r="E243">
+        <v>180</v>
+      </c>
+      <c r="F243" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>249</v>
+      </c>
+      <c r="B244">
+        <v>9</v>
+      </c>
+      <c r="C244">
+        <v>9</v>
+      </c>
+      <c r="D244">
+        <v>10</v>
+      </c>
+      <c r="E244">
+        <v>810</v>
+      </c>
+      <c r="F244" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>250</v>
+      </c>
+      <c r="B245">
+        <v>5</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
+      <c r="D245">
+        <v>2</v>
+      </c>
+      <c r="E245">
+        <v>10</v>
+      </c>
+      <c r="F245" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>251</v>
+      </c>
+      <c r="B246">
+        <v>8</v>
+      </c>
+      <c r="C246">
+        <v>9</v>
+      </c>
+      <c r="D246">
+        <v>4</v>
+      </c>
+      <c r="E246">
+        <v>288</v>
+      </c>
+      <c r="F246" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>252</v>
+      </c>
+      <c r="B247">
+        <v>6</v>
+      </c>
+      <c r="C247">
+        <v>2</v>
+      </c>
+      <c r="D247">
+        <v>2</v>
+      </c>
+      <c r="E247">
+        <v>24</v>
+      </c>
+      <c r="F247" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>253</v>
+      </c>
+      <c r="B248">
+        <v>2</v>
+      </c>
+      <c r="C248">
+        <v>3</v>
+      </c>
+      <c r="D248">
+        <v>2</v>
+      </c>
+      <c r="E248">
+        <v>12</v>
+      </c>
+      <c r="F248" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>254</v>
+      </c>
+      <c r="B249">
+        <v>2</v>
+      </c>
+      <c r="C249">
+        <v>3</v>
+      </c>
+      <c r="D249">
+        <v>9</v>
+      </c>
+      <c r="E249">
+        <v>54</v>
+      </c>
+      <c r="F249" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>255</v>
+      </c>
+      <c r="B250">
+        <v>9</v>
+      </c>
+      <c r="C250">
+        <v>3</v>
+      </c>
+      <c r="D250">
+        <v>3</v>
+      </c>
+      <c r="E250">
+        <v>81</v>
+      </c>
+      <c r="F250" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>314</v>
+      </c>
+      <c r="B251">
+        <v>7</v>
+      </c>
+      <c r="C251">
+        <v>5</v>
+      </c>
+      <c r="D251">
+        <v>1</v>
+      </c>
+      <c r="E251">
+        <v>35</v>
+      </c>
+      <c r="F251" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>256</v>
+      </c>
+      <c r="B252">
+        <v>8</v>
+      </c>
+      <c r="C252">
+        <v>9</v>
+      </c>
+      <c r="D252">
+        <v>1</v>
+      </c>
+      <c r="E252">
+        <v>72</v>
+      </c>
+      <c r="F252" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>257</v>
+      </c>
+      <c r="B253">
+        <v>4</v>
+      </c>
+      <c r="C253">
+        <v>1</v>
+      </c>
+      <c r="D253">
+        <v>5</v>
+      </c>
+      <c r="E253">
+        <v>20</v>
+      </c>
+      <c r="F253" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>258</v>
+      </c>
+      <c r="B254">
+        <v>8</v>
+      </c>
+      <c r="C254">
+        <v>10</v>
+      </c>
+      <c r="D254">
+        <v>3</v>
+      </c>
+      <c r="E254">
+        <v>240</v>
+      </c>
+      <c r="F254" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>259</v>
+      </c>
+      <c r="B255">
+        <v>10</v>
+      </c>
+      <c r="C255">
+        <v>6</v>
+      </c>
+      <c r="D255">
+        <v>4</v>
+      </c>
+      <c r="E255">
+        <v>240</v>
+      </c>
+      <c r="F255" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>260</v>
+      </c>
+      <c r="B256">
+        <v>2</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
+      <c r="D256">
+        <v>8</v>
+      </c>
+      <c r="E256">
+        <v>16</v>
+      </c>
+      <c r="F256" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>261</v>
+      </c>
+      <c r="B257">
+        <v>3</v>
+      </c>
+      <c r="C257">
+        <v>5</v>
+      </c>
+      <c r="D257">
+        <v>10</v>
+      </c>
+      <c r="E257">
+        <v>150</v>
+      </c>
+      <c r="F257" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>262</v>
+      </c>
+      <c r="B258">
+        <v>3</v>
+      </c>
+      <c r="C258">
+        <v>6</v>
+      </c>
+      <c r="D258">
+        <v>2</v>
+      </c>
+      <c r="E258">
+        <v>36</v>
+      </c>
+      <c r="F258" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>263</v>
+      </c>
+      <c r="B259">
+        <v>3</v>
+      </c>
+      <c r="C259">
+        <v>6</v>
+      </c>
+      <c r="D259">
+        <v>10</v>
+      </c>
+      <c r="E259">
+        <v>180</v>
+      </c>
+      <c r="F259" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>264</v>
+      </c>
+      <c r="B260">
+        <v>4</v>
+      </c>
+      <c r="C260">
+        <v>10</v>
+      </c>
+      <c r="D260">
+        <v>9</v>
+      </c>
+      <c r="E260">
+        <v>360</v>
+      </c>
+      <c r="F260" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>265</v>
+      </c>
+      <c r="B261">
+        <v>3</v>
+      </c>
+      <c r="C261">
+        <v>2</v>
+      </c>
+      <c r="D261">
+        <v>7</v>
+      </c>
+      <c r="E261">
+        <v>42</v>
+      </c>
+      <c r="F261" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>34</v>
+      </c>
+      <c r="B262">
+        <v>5</v>
+      </c>
+      <c r="C262">
+        <v>4</v>
+      </c>
+      <c r="D262">
+        <v>7</v>
+      </c>
+      <c r="E262">
+        <v>140</v>
+      </c>
+      <c r="F262" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>266</v>
+      </c>
+      <c r="B263">
+        <v>1</v>
+      </c>
+      <c r="C263">
+        <v>2</v>
+      </c>
+      <c r="D263">
+        <v>3</v>
+      </c>
+      <c r="E263">
+        <v>6</v>
+      </c>
+      <c r="F263" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>315</v>
+      </c>
+      <c r="B264">
+        <v>9</v>
+      </c>
+      <c r="C264">
+        <v>7</v>
+      </c>
+      <c r="D264">
+        <v>5</v>
+      </c>
+      <c r="E264">
+        <v>315</v>
+      </c>
+      <c r="F264" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>267</v>
+      </c>
+      <c r="B265">
+        <v>1</v>
+      </c>
+      <c r="C265">
+        <v>5</v>
+      </c>
+      <c r="D265">
+        <v>6</v>
+      </c>
+      <c r="E265">
+        <v>30</v>
+      </c>
+      <c r="F265" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>268</v>
+      </c>
+      <c r="B266">
+        <v>4</v>
+      </c>
+      <c r="C266">
+        <v>10</v>
+      </c>
+      <c r="D266">
+        <v>2</v>
+      </c>
+      <c r="E266">
+        <v>80</v>
+      </c>
+      <c r="F266" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>269</v>
+      </c>
+      <c r="B267">
+        <v>6</v>
+      </c>
+      <c r="C267">
+        <v>8</v>
+      </c>
+      <c r="D267">
+        <v>8</v>
+      </c>
+      <c r="E267">
+        <v>384</v>
+      </c>
+      <c r="F267" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>270</v>
+      </c>
+      <c r="B268">
+        <v>9</v>
+      </c>
+      <c r="C268">
+        <v>7</v>
+      </c>
+      <c r="D268">
+        <v>1</v>
+      </c>
+      <c r="E268">
+        <v>63</v>
+      </c>
+      <c r="F268" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>316</v>
+      </c>
+      <c r="B269">
+        <v>10</v>
+      </c>
+      <c r="C269">
+        <v>7</v>
+      </c>
+      <c r="D269">
+        <v>9</v>
+      </c>
+      <c r="E269">
+        <v>630</v>
+      </c>
+      <c r="F269" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>271</v>
+      </c>
+      <c r="B270">
+        <v>1</v>
+      </c>
+      <c r="C270">
+        <v>8</v>
+      </c>
+      <c r="D270">
+        <v>2</v>
+      </c>
+      <c r="E270">
+        <v>16</v>
+      </c>
+      <c r="F270" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>272</v>
+      </c>
+      <c r="B271">
+        <v>6</v>
+      </c>
+      <c r="C271">
+        <v>3</v>
+      </c>
+      <c r="D271">
+        <v>8</v>
+      </c>
+      <c r="E271">
+        <v>144</v>
+      </c>
+      <c r="F271" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>273</v>
+      </c>
+      <c r="B272" s="4">
+        <v>10</v>
+      </c>
+      <c r="C272">
+        <v>6</v>
+      </c>
+      <c r="D272">
+        <v>3</v>
+      </c>
+      <c r="E272">
+        <v>180</v>
+      </c>
+      <c r="F272" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>274</v>
+      </c>
+      <c r="B273">
+        <v>1</v>
+      </c>
+      <c r="C273">
+        <v>9</v>
+      </c>
+      <c r="D273">
+        <v>9</v>
+      </c>
+      <c r="E273">
+        <v>81</v>
+      </c>
+      <c r="F273" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>317</v>
+      </c>
+      <c r="B274">
+        <v>1</v>
+      </c>
+      <c r="C274">
+        <v>5</v>
+      </c>
+      <c r="D274">
+        <v>10</v>
+      </c>
+      <c r="E274">
+        <v>50</v>
+      </c>
+      <c r="F274" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>275</v>
+      </c>
+      <c r="B275">
+        <v>9</v>
+      </c>
+      <c r="C275">
+        <v>8</v>
+      </c>
+      <c r="D275">
+        <v>4</v>
+      </c>
+      <c r="E275">
+        <v>288</v>
+      </c>
+      <c r="F275" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>276</v>
+      </c>
+      <c r="B276">
+        <v>6</v>
+      </c>
+      <c r="C276">
+        <v>9</v>
+      </c>
+      <c r="D276">
+        <v>6</v>
+      </c>
+      <c r="E276">
+        <v>324</v>
+      </c>
+      <c r="F276" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>277</v>
+      </c>
+      <c r="B277">
+        <v>8</v>
+      </c>
+      <c r="C277">
+        <v>8</v>
+      </c>
+      <c r="D277">
+        <v>8</v>
+      </c>
+      <c r="E277">
+        <v>512</v>
+      </c>
+      <c r="F277" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>278</v>
+      </c>
+      <c r="B278">
+        <v>3</v>
+      </c>
+      <c r="C278">
+        <v>8</v>
+      </c>
+      <c r="D278">
+        <v>2</v>
+      </c>
+      <c r="E278">
+        <v>48</v>
+      </c>
+      <c r="F278" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>279</v>
+      </c>
+      <c r="B279">
+        <v>9</v>
+      </c>
+      <c r="C279">
+        <v>3</v>
+      </c>
+      <c r="D279">
+        <v>4</v>
+      </c>
+      <c r="E279">
+        <v>108</v>
+      </c>
+      <c r="F279" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>318</v>
+      </c>
+      <c r="B280">
+        <v>4</v>
+      </c>
+      <c r="C280">
+        <v>9</v>
+      </c>
+      <c r="D280">
+        <v>7</v>
+      </c>
+      <c r="E280">
+        <v>252</v>
+      </c>
+      <c r="F280" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>280</v>
+      </c>
+      <c r="B281">
+        <v>5</v>
+      </c>
+      <c r="C281">
+        <v>10</v>
+      </c>
+      <c r="D281">
+        <v>2</v>
+      </c>
+      <c r="E281">
+        <v>100</v>
+      </c>
+      <c r="F281" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>281</v>
+      </c>
+      <c r="B282">
+        <v>1</v>
+      </c>
+      <c r="C282">
+        <v>1</v>
+      </c>
+      <c r="D282">
+        <v>8</v>
+      </c>
+      <c r="E282">
+        <v>8</v>
+      </c>
+      <c r="F282" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>282</v>
+      </c>
+      <c r="B283">
+        <v>2</v>
+      </c>
+      <c r="C283">
+        <v>6</v>
+      </c>
+      <c r="D283">
+        <v>1</v>
+      </c>
+      <c r="E283">
+        <v>12</v>
+      </c>
+      <c r="F283" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>283</v>
+      </c>
+      <c r="B284">
+        <v>7</v>
+      </c>
+      <c r="C284">
+        <v>4</v>
+      </c>
+      <c r="D284">
+        <v>10</v>
+      </c>
+      <c r="E284">
+        <v>280</v>
+      </c>
+      <c r="F284" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>285</v>
+      </c>
+      <c r="B285">
+        <v>10</v>
+      </c>
+      <c r="C285">
+        <v>10</v>
+      </c>
+      <c r="D285">
+        <v>5</v>
+      </c>
+      <c r="E285">
+        <v>500</v>
+      </c>
+      <c r="F285" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>286</v>
+      </c>
+      <c r="B286">
+        <v>4</v>
+      </c>
+      <c r="C286">
+        <v>4</v>
+      </c>
+      <c r="D286">
+        <v>2</v>
+      </c>
+      <c r="E286">
+        <v>32</v>
+      </c>
+      <c r="F286" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>135</v>
+      </c>
+      <c r="B287">
+        <v>7</v>
+      </c>
+      <c r="C287">
+        <v>4</v>
+      </c>
+      <c r="D287">
+        <v>1</v>
+      </c>
+      <c r="E287">
+        <v>28</v>
+      </c>
+      <c r="F287" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>287</v>
+      </c>
+      <c r="B288">
+        <v>8</v>
+      </c>
+      <c r="C288">
+        <v>7</v>
+      </c>
+      <c r="D288">
+        <v>4</v>
+      </c>
+      <c r="E288">
+        <v>224</v>
+      </c>
+      <c r="F288" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>288</v>
+      </c>
+      <c r="B289">
+        <v>3</v>
+      </c>
+      <c r="C289">
+        <v>1</v>
+      </c>
+      <c r="D289">
+        <v>9</v>
+      </c>
+      <c r="E289">
+        <v>27</v>
+      </c>
+      <c r="F289" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>289</v>
+      </c>
+      <c r="B290">
+        <v>3</v>
+      </c>
+      <c r="C290">
+        <v>7</v>
+      </c>
+      <c r="D290">
+        <v>3</v>
+      </c>
+      <c r="E290">
+        <v>63</v>
+      </c>
+      <c r="F290" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>319</v>
+      </c>
+      <c r="B291">
+        <v>7</v>
+      </c>
+      <c r="C291">
+        <v>4</v>
+      </c>
+      <c r="D291">
+        <v>4</v>
+      </c>
+      <c r="E291">
+        <v>112</v>
+      </c>
+      <c r="F291" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>290</v>
+      </c>
+      <c r="B292">
+        <v>10</v>
+      </c>
+      <c r="C292">
+        <v>6</v>
+      </c>
+      <c r="D292">
+        <v>7</v>
+      </c>
+      <c r="E292">
+        <v>420</v>
+      </c>
+      <c r="F292" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>21</v>
+      </c>
+      <c r="B293">
+        <v>4</v>
+      </c>
+      <c r="C293">
+        <v>8</v>
+      </c>
+      <c r="D293">
+        <v>3</v>
+      </c>
+      <c r="E293">
+        <v>96</v>
+      </c>
+      <c r="F293" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>291</v>
+      </c>
+      <c r="B294">
+        <v>5</v>
+      </c>
+      <c r="C294">
+        <v>9</v>
+      </c>
+      <c r="D294">
+        <v>3</v>
+      </c>
+      <c r="E294">
+        <v>135</v>
+      </c>
+      <c r="F294" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>292</v>
+      </c>
+      <c r="B295">
+        <v>1</v>
+      </c>
+      <c r="C295">
+        <v>6</v>
+      </c>
+      <c r="D295">
+        <v>9</v>
+      </c>
+      <c r="E295">
+        <v>54</v>
+      </c>
+      <c r="F295" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>294</v>
+      </c>
+      <c r="B296">
+        <v>4</v>
+      </c>
+      <c r="C296">
+        <v>8</v>
+      </c>
+      <c r="D296">
+        <v>5</v>
+      </c>
+      <c r="E296">
+        <v>160</v>
+      </c>
+      <c r="F296" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>320</v>
+      </c>
+      <c r="B297">
+        <v>3</v>
+      </c>
+      <c r="C297">
+        <v>8</v>
+      </c>
+      <c r="D297">
+        <v>4</v>
+      </c>
+      <c r="E297">
+        <v>96</v>
+      </c>
+      <c r="F297" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>295</v>
+      </c>
+      <c r="B298">
+        <v>4</v>
+      </c>
+      <c r="C298">
+        <v>6</v>
+      </c>
+      <c r="D298">
+        <v>10</v>
+      </c>
+      <c r="E298">
+        <v>240</v>
+      </c>
+      <c r="F298" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>229</v>
+      </c>
+      <c r="B299">
+        <v>9</v>
+      </c>
+      <c r="C299">
+        <v>6</v>
+      </c>
+      <c r="D299">
+        <v>5</v>
+      </c>
+      <c r="E299">
+        <v>270</v>
+      </c>
+      <c r="F299" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>296</v>
+      </c>
+      <c r="B300">
+        <v>9</v>
+      </c>
+      <c r="C300">
+        <v>5</v>
+      </c>
+      <c r="D300">
+        <v>5</v>
+      </c>
+      <c r="E300">
+        <v>225</v>
+      </c>
+      <c r="F300" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>297</v>
+      </c>
+      <c r="B301">
+        <v>4</v>
+      </c>
+      <c r="C301">
+        <v>5</v>
+      </c>
+      <c r="D301">
+        <v>2</v>
+      </c>
+      <c r="E301">
+        <v>40</v>
+      </c>
+      <c r="F301" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>298</v>
+      </c>
+      <c r="B302">
+        <v>3</v>
+      </c>
+      <c r="C302">
+        <v>9</v>
+      </c>
+      <c r="D302">
+        <v>1</v>
+      </c>
+      <c r="E302">
+        <v>27</v>
+      </c>
+      <c r="F302" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>299</v>
+      </c>
+      <c r="B303">
+        <v>2</v>
+      </c>
+      <c r="C303">
+        <v>7</v>
+      </c>
+      <c r="D303">
+        <v>9</v>
+      </c>
+      <c r="E303">
+        <v>126</v>
+      </c>
+      <c r="F303" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>300</v>
+      </c>
+      <c r="B304">
+        <v>10</v>
+      </c>
+      <c r="C304">
+        <v>2</v>
+      </c>
+      <c r="D304">
+        <v>7</v>
+      </c>
+      <c r="E304">
+        <v>140</v>
+      </c>
+      <c r="F304" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>301</v>
+      </c>
+      <c r="B305">
+        <v>4</v>
+      </c>
+      <c r="C305">
+        <v>6</v>
+      </c>
+      <c r="D305">
+        <v>4</v>
+      </c>
+      <c r="E305">
+        <v>96</v>
+      </c>
+      <c r="F305" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>302</v>
+      </c>
+      <c r="B306">
+        <v>10</v>
+      </c>
+      <c r="C306">
+        <v>1</v>
+      </c>
+      <c r="D306">
+        <v>7</v>
+      </c>
+      <c r="E306">
+        <v>70</v>
+      </c>
+      <c r="F306" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>303</v>
+      </c>
+      <c r="B307">
+        <v>3</v>
+      </c>
+      <c r="C307">
+        <v>6</v>
+      </c>
+      <c r="D307">
+        <v>4</v>
+      </c>
+      <c r="E307">
+        <v>72</v>
+      </c>
+      <c r="F307" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>305</v>
+      </c>
+      <c r="B308">
+        <v>5</v>
+      </c>
+      <c r="C308">
+        <v>8</v>
+      </c>
+      <c r="D308">
+        <v>2</v>
+      </c>
+      <c r="E308">
+        <v>80</v>
+      </c>
+      <c r="F308" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>306</v>
+      </c>
+      <c r="B309">
+        <v>9</v>
+      </c>
+      <c r="C309">
+        <v>8</v>
+      </c>
+      <c r="D309">
+        <v>1</v>
+      </c>
+      <c r="E309">
+        <v>72</v>
+      </c>
+      <c r="F309" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>307</v>
+      </c>
+      <c r="B310" s="4">
+        <v>6</v>
+      </c>
+      <c r="C310">
+        <v>9</v>
+      </c>
+      <c r="D310">
+        <v>5</v>
+      </c>
+      <c r="E310">
+        <v>270</v>
+      </c>
+      <c r="F310" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>308</v>
+      </c>
+      <c r="B311" s="4">
+        <v>9</v>
+      </c>
+      <c r="C311">
+        <v>9</v>
+      </c>
+      <c r="D311">
+        <v>7</v>
+      </c>
+      <c r="E311">
+        <v>567</v>
+      </c>
+      <c r="F311" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>309</v>
+      </c>
+      <c r="B312" s="4">
+        <v>6</v>
+      </c>
+      <c r="C312">
+        <v>7</v>
+      </c>
+      <c r="D312">
+        <v>9</v>
+      </c>
+      <c r="E312">
+        <v>378</v>
+      </c>
+      <c r="F312" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A313" t="s">
+        <v>310</v>
+      </c>
+      <c r="B313" s="4">
+        <v>1</v>
+      </c>
+      <c r="C313">
+        <v>6</v>
+      </c>
+      <c r="D313">
+        <v>5</v>
+      </c>
+      <c r="E313">
+        <v>30</v>
+      </c>
+      <c r="F313" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>119</v>
+      </c>
+      <c r="B314" s="4">
+        <v>8</v>
+      </c>
+      <c r="C314">
+        <v>1</v>
+      </c>
+      <c r="D314">
+        <v>3</v>
+      </c>
+      <c r="E314">
+        <v>24</v>
+      </c>
+      <c r="F314" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>311</v>
+      </c>
+      <c r="B315">
+        <v>8</v>
+      </c>
+      <c r="C315">
+        <v>1</v>
+      </c>
+      <c r="D315">
+        <v>3</v>
+      </c>
+      <c r="E315">
+        <v>24</v>
+      </c>
+      <c r="F315" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>284</v>
+      </c>
+      <c r="B316">
+        <v>9</v>
+      </c>
+      <c r="C316">
+        <v>6</v>
+      </c>
+      <c r="D316">
+        <v>7</v>
+      </c>
+      <c r="E316">
+        <v>378</v>
+      </c>
+      <c r="F316" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
+        <v>293</v>
+      </c>
+      <c r="B317">
+        <v>8</v>
+      </c>
+      <c r="C317">
+        <v>3</v>
+      </c>
+      <c r="D317">
+        <v>2</v>
+      </c>
+      <c r="E317">
+        <v>48</v>
+      </c>
+      <c r="F317" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
+        <v>304</v>
+      </c>
+      <c r="B318">
+        <v>1</v>
+      </c>
+      <c r="C318">
+        <v>3</v>
+      </c>
+      <c r="D318">
+        <v>5</v>
+      </c>
+      <c r="E318">
+        <v>15</v>
+      </c>
+      <c r="F318" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added RPN.xlsx for deployment
</commit_message>
<xml_diff>
--- a/ProcessedData/RPN.xlsx
+++ b/ProcessedData/RPN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KOEL\ICSS\Deployment\icss-backend\ProcessedData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KOEL\ICSS\Deployment\icss-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD40280-1F6A-4E67-9946-3B504338A09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7A2F25-1E43-4744-A91D-6B96B1F09BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="193">
   <si>
     <t>Severity (S)</t>
   </si>
@@ -604,390 +604,6 @@
   </si>
   <si>
     <t>Exhaust Manifold</t>
-  </si>
-  <si>
-    <t>LLOP</t>
-  </si>
-  <si>
-    <t>Earth Control Valve</t>
-  </si>
-  <si>
-    <t>Fuse Failure</t>
-  </si>
-  <si>
-    <t>Oil Leakage</t>
-  </si>
-  <si>
-    <t>Oil Drain</t>
-  </si>
-  <si>
-    <t>Exhaust Conical Filter</t>
-  </si>
-  <si>
-    <t>Panel Wiring</t>
-  </si>
-  <si>
-    <t>Silencer</t>
-  </si>
-  <si>
-    <t>Emergency Switch</t>
-  </si>
-  <si>
-    <t>Emergency Stop Button</t>
-  </si>
-  <si>
-    <t>V-Belt</t>
-  </si>
-  <si>
-    <t>Sump</t>
-  </si>
-  <si>
-    <t>Carburettor</t>
-  </si>
-  <si>
-    <t>Exhaust Silencer Flange</t>
-  </si>
-  <si>
-    <t>Hose Clip</t>
-  </si>
-  <si>
-    <t>VMR</t>
-  </si>
-  <si>
-    <t>RPM</t>
-  </si>
-  <si>
-    <t>Mains</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Adblue</t>
-  </si>
-  <si>
-    <t>Alarm</t>
-  </si>
-  <si>
-    <t>Washer</t>
-  </si>
-  <si>
-    <t>Airlock</t>
-  </si>
-  <si>
-    <t>Bellow</t>
-  </si>
-  <si>
-    <t>Rocker Cover</t>
-  </si>
-  <si>
-    <t>T6 Sensor</t>
-  </si>
-  <si>
-    <t>Lube Oil Pressure</t>
-  </si>
-  <si>
-    <t>Exhaust Gas Recirculation</t>
-  </si>
-  <si>
-    <t>Super Capacitor</t>
-  </si>
-  <si>
-    <t>Self-Starter</t>
-  </si>
-  <si>
-    <t>Breather</t>
-  </si>
-  <si>
-    <t>clamp</t>
-  </si>
-  <si>
-    <t>Dipstick</t>
-  </si>
-  <si>
-    <t>Inverter Module</t>
-  </si>
-  <si>
-    <t>Solenoid</t>
-  </si>
-  <si>
-    <t>Engine Hunting</t>
-  </si>
-  <si>
-    <t>Gasket</t>
-  </si>
-  <si>
-    <t>Synchronisation</t>
-  </si>
-  <si>
-    <t>Engine Crank</t>
-  </si>
-  <si>
-    <t>Diesel Leakage</t>
-  </si>
-  <si>
-    <t>AVR</t>
-  </si>
-  <si>
-    <t>Oil Sensor</t>
-  </si>
-  <si>
-    <t>Voltage fluctutation</t>
-  </si>
-  <si>
-    <t>Low Voltage</t>
-  </si>
-  <si>
-    <t>silencer Glading</t>
-  </si>
-  <si>
-    <t>Lug</t>
-  </si>
-  <si>
-    <t>Control Selector</t>
-  </si>
-  <si>
-    <t>Sweep Stuck Alarm</t>
-  </si>
-  <si>
-    <t>CT Neutral</t>
-  </si>
-  <si>
-    <t>Gauge</t>
-  </si>
-  <si>
-    <t>AMF</t>
-  </si>
-  <si>
-    <t>Gas Pressure</t>
-  </si>
-  <si>
-    <t>chock</t>
-  </si>
-  <si>
-    <t>Crank Case</t>
-  </si>
-  <si>
-    <t>Gear Casing</t>
-  </si>
-  <si>
-    <t>Union Thread</t>
-  </si>
-  <si>
-    <t>Adapter</t>
-  </si>
-  <si>
-    <t>MPU</t>
-  </si>
-  <si>
-    <t>Seepage</t>
-  </si>
-  <si>
-    <t>CAC hose</t>
-  </si>
-  <si>
-    <t>Ferule</t>
-  </si>
-  <si>
-    <t>Abnormal</t>
-  </si>
-  <si>
-    <t>DOC</t>
-  </si>
-  <si>
-    <t>Flashing</t>
-  </si>
-  <si>
-    <t>Reverse Power Alarm</t>
-  </si>
-  <si>
-    <t>Banjo</t>
-  </si>
-  <si>
-    <t>Feed Pump</t>
-  </si>
-  <si>
-    <t>Belt Tensioner Meter</t>
-  </si>
-  <si>
-    <t>Ignition Switch</t>
-  </si>
-  <si>
-    <t>Crank Speed Sensor</t>
-  </si>
-  <si>
-    <t>Selector Switch</t>
-  </si>
-  <si>
-    <t>Armature</t>
-  </si>
-  <si>
-    <t>Piston</t>
-  </si>
-  <si>
-    <t>FIP</t>
-  </si>
-  <si>
-    <t>Idle Gear</t>
-  </si>
-  <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>Urea Dosing</t>
-  </si>
-  <si>
-    <t>Lube Oil Leakage</t>
-  </si>
-  <si>
-    <t>Allen Key</t>
-  </si>
-  <si>
-    <t>Contactor</t>
-  </si>
-  <si>
-    <t>Turbo Charger</t>
-  </si>
-  <si>
-    <t>Canopy</t>
-  </si>
-  <si>
-    <t>Temperature Switch</t>
-  </si>
-  <si>
-    <t>Control panel</t>
-  </si>
-  <si>
-    <t>Line rejection</t>
-  </si>
-  <si>
-    <t>Fan Pulley</t>
-  </si>
-  <si>
-    <t>Gas filter</t>
-  </si>
-  <si>
-    <t>Bolt</t>
-  </si>
-  <si>
-    <t>ITV</t>
-  </si>
-  <si>
-    <t>Eye Bolt</t>
-  </si>
-  <si>
-    <t>Compressor</t>
-  </si>
-  <si>
-    <t>Fuel Rack</t>
-  </si>
-  <si>
-    <t>Nozzle</t>
-  </si>
-  <si>
-    <t>Valve Bridge</t>
-  </si>
-  <si>
-    <t>MCCB</t>
-  </si>
-  <si>
-    <t>Pump</t>
-  </si>
-  <si>
-    <t>PRV</t>
-  </si>
-  <si>
-    <t>Electric Feed Pump</t>
-  </si>
-  <si>
-    <t>Regulator</t>
-  </si>
-  <si>
-    <t>Exhaust Pipe</t>
-  </si>
-  <si>
-    <t>CT Transformer</t>
-  </si>
-  <si>
-    <t>Engine Block</t>
-  </si>
-  <si>
-    <t>LED Flickering</t>
-  </si>
-  <si>
-    <t>CNC Machine</t>
-  </si>
-  <si>
-    <t>LVM</t>
-  </si>
-  <si>
-    <t>DCU</t>
-  </si>
-  <si>
-    <t>Auto Sensing Cable</t>
-  </si>
-  <si>
-    <t>CAC Pipe</t>
-  </si>
-  <si>
-    <t>Amber Lamp</t>
-  </si>
-  <si>
-    <t>Muffler</t>
-  </si>
-  <si>
-    <t>Stuck Float</t>
-  </si>
-  <si>
-    <t>Fuel float valve</t>
-  </si>
-  <si>
-    <t>Common Rail</t>
-  </si>
-  <si>
-    <t>Sensor</t>
-  </si>
-  <si>
-    <t>DPF Weight Measurement</t>
-  </si>
-  <si>
-    <t>Rotor</t>
-  </si>
-  <si>
-    <t>Flash Protect Lamp</t>
-  </si>
-  <si>
-    <t>Governor Spring Pad</t>
-  </si>
-  <si>
-    <t>EMS Switch</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>o-ring</t>
-  </si>
-  <si>
-    <t>Fan Belt</t>
-  </si>
-  <si>
-    <t>Fuel Filter</t>
-  </si>
-  <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>Tappet</t>
-  </si>
-  <si>
-    <t>Spark Arrestor</t>
-  </si>
-  <si>
-    <t>Regeneration</t>
-  </si>
-  <si>
-    <t>Capacitor</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1042,7 +658,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1323,15 +938,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F318"/>
+  <dimension ref="A1:F186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
-      <selection activeCell="A320" sqref="A320"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.21875" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
@@ -2038,7 +1653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>82</v>
       </c>
@@ -2058,7 +1673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>83</v>
       </c>
@@ -2118,7 +1733,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
@@ -2138,7 +1753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
@@ -2158,7 +1773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
@@ -2178,7 +1793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>86</v>
       </c>
@@ -2198,7 +1813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>87</v>
       </c>
@@ -2438,7 +2053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>99</v>
       </c>
@@ -2498,7 +2113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>40</v>
       </c>
@@ -2558,7 +2173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>103</v>
       </c>
@@ -2578,7 +2193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
@@ -2598,7 +2213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>105</v>
       </c>
@@ -2618,7 +2233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>106</v>
       </c>
@@ -2638,7 +2253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>107</v>
       </c>
@@ -2718,7 +2333,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>108</v>
       </c>
@@ -2738,7 +2353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>46</v>
       </c>
@@ -2858,7 +2473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>109</v>
       </c>
@@ -2898,7 +2513,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>52</v>
       </c>
@@ -2938,7 +2553,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>53</v>
       </c>
@@ -2978,7 +2593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>111</v>
       </c>
@@ -3038,7 +2653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>114</v>
       </c>
@@ -3058,7 +2673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>115</v>
       </c>
@@ -3298,7 +2913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>120</v>
       </c>
@@ -3318,7 +2933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>121</v>
       </c>
@@ -3338,7 +2953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>122</v>
       </c>
@@ -3358,7 +2973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>123</v>
       </c>
@@ -3418,7 +3033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>126</v>
       </c>
@@ -3478,7 +3093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>129</v>
       </c>
@@ -3558,7 +3173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>133</v>
       </c>
@@ -3578,7 +3193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>134</v>
       </c>
@@ -3638,7 +3253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>137</v>
       </c>
@@ -3658,7 +3273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>138</v>
       </c>
@@ -3678,7 +3293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>139</v>
       </c>
@@ -3698,7 +3313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>140</v>
       </c>
@@ -3718,7 +3333,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>141</v>
       </c>
@@ -3738,7 +3353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>142</v>
       </c>
@@ -3758,7 +3373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>143</v>
       </c>
@@ -3818,7 +3433,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>66</v>
       </c>
@@ -3858,7 +3473,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>68</v>
       </c>
@@ -4038,7 +3653,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>144</v>
       </c>
@@ -4218,7 +3833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>153</v>
       </c>
@@ -4238,7 +3853,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>154</v>
       </c>
@@ -4258,7 +3873,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>155</v>
       </c>
@@ -4278,7 +3893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>156</v>
       </c>
@@ -4298,7 +3913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>157</v>
       </c>
@@ -4318,7 +3933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>158</v>
       </c>
@@ -4338,7 +3953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>159</v>
       </c>
@@ -4358,7 +3973,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>160</v>
       </c>
@@ -4398,7 +4013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>161</v>
       </c>
@@ -4418,7 +4033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>120</v>
       </c>
@@ -4438,7 +4053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>162</v>
       </c>
@@ -4458,7 +4073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>163</v>
       </c>
@@ -4578,7 +4193,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>169</v>
       </c>
@@ -5038,7 +4653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>192</v>
       </c>
@@ -5056,2646 +4671,6 @@
       </c>
       <c r="F186" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
-        <v>193</v>
-      </c>
-      <c r="B187">
-        <v>1</v>
-      </c>
-      <c r="C187">
-        <v>4</v>
-      </c>
-      <c r="D187">
-        <v>10</v>
-      </c>
-      <c r="E187">
-        <v>40</v>
-      </c>
-      <c r="F187" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
-        <v>194</v>
-      </c>
-      <c r="B188">
-        <v>1</v>
-      </c>
-      <c r="C188">
-        <v>10</v>
-      </c>
-      <c r="D188">
-        <v>2</v>
-      </c>
-      <c r="E188">
-        <v>20</v>
-      </c>
-      <c r="F188" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
-        <v>195</v>
-      </c>
-      <c r="B189">
-        <v>1</v>
-      </c>
-      <c r="C189">
-        <v>5</v>
-      </c>
-      <c r="D189">
-        <v>4</v>
-      </c>
-      <c r="E189">
-        <v>20</v>
-      </c>
-      <c r="F189" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
-        <v>196</v>
-      </c>
-      <c r="B190">
-        <v>2</v>
-      </c>
-      <c r="C190">
-        <v>5</v>
-      </c>
-      <c r="D190">
-        <v>9</v>
-      </c>
-      <c r="E190">
-        <v>90</v>
-      </c>
-      <c r="F190" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
-        <v>197</v>
-      </c>
-      <c r="B191">
-        <v>4</v>
-      </c>
-      <c r="C191">
-        <v>3</v>
-      </c>
-      <c r="D191">
-        <v>9</v>
-      </c>
-      <c r="E191">
-        <v>108</v>
-      </c>
-      <c r="F191" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A192" t="s">
-        <v>198</v>
-      </c>
-      <c r="B192">
-        <v>3</v>
-      </c>
-      <c r="C192">
-        <v>4</v>
-      </c>
-      <c r="D192">
-        <v>4</v>
-      </c>
-      <c r="E192">
-        <v>48</v>
-      </c>
-      <c r="F192" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A193" t="s">
-        <v>199</v>
-      </c>
-      <c r="B193">
-        <v>10</v>
-      </c>
-      <c r="C193">
-        <v>8</v>
-      </c>
-      <c r="D193">
-        <v>5</v>
-      </c>
-      <c r="E193">
-        <v>400</v>
-      </c>
-      <c r="F193" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A194" t="s">
-        <v>200</v>
-      </c>
-      <c r="B194">
-        <v>3</v>
-      </c>
-      <c r="C194">
-        <v>10</v>
-      </c>
-      <c r="D194">
-        <v>9</v>
-      </c>
-      <c r="E194">
-        <v>270</v>
-      </c>
-      <c r="F194" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A195" t="s">
-        <v>201</v>
-      </c>
-      <c r="B195">
-        <v>6</v>
-      </c>
-      <c r="C195">
-        <v>10</v>
-      </c>
-      <c r="D195">
-        <v>9</v>
-      </c>
-      <c r="E195">
-        <v>540</v>
-      </c>
-      <c r="F195" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
-        <v>202</v>
-      </c>
-      <c r="B196">
-        <v>8</v>
-      </c>
-      <c r="C196">
-        <v>5</v>
-      </c>
-      <c r="D196">
-        <v>5</v>
-      </c>
-      <c r="E196">
-        <v>200</v>
-      </c>
-      <c r="F196" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A197" t="s">
-        <v>313</v>
-      </c>
-      <c r="B197">
-        <v>10</v>
-      </c>
-      <c r="C197">
-        <v>10</v>
-      </c>
-      <c r="D197">
-        <v>1</v>
-      </c>
-      <c r="E197">
-        <v>100</v>
-      </c>
-      <c r="F197" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A198" t="s">
-        <v>203</v>
-      </c>
-      <c r="B198">
-        <v>10</v>
-      </c>
-      <c r="C198">
-        <v>1</v>
-      </c>
-      <c r="D198">
-        <v>3</v>
-      </c>
-      <c r="E198">
-        <v>30</v>
-      </c>
-      <c r="F198" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A199" t="s">
-        <v>204</v>
-      </c>
-      <c r="B199">
-        <v>1</v>
-      </c>
-      <c r="C199">
-        <v>5</v>
-      </c>
-      <c r="D199">
-        <v>2</v>
-      </c>
-      <c r="E199">
-        <v>10</v>
-      </c>
-      <c r="F199" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
-        <v>205</v>
-      </c>
-      <c r="B200">
-        <v>1</v>
-      </c>
-      <c r="C200">
-        <v>1</v>
-      </c>
-      <c r="D200">
-        <v>7</v>
-      </c>
-      <c r="E200">
-        <v>7</v>
-      </c>
-      <c r="F200" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
-        <v>206</v>
-      </c>
-      <c r="B201">
-        <v>2</v>
-      </c>
-      <c r="C201">
-        <v>2</v>
-      </c>
-      <c r="D201">
-        <v>7</v>
-      </c>
-      <c r="E201">
-        <v>28</v>
-      </c>
-      <c r="F201" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
-        <v>207</v>
-      </c>
-      <c r="B202">
-        <v>2</v>
-      </c>
-      <c r="C202">
-        <v>6</v>
-      </c>
-      <c r="D202">
-        <v>5</v>
-      </c>
-      <c r="E202">
-        <v>60</v>
-      </c>
-      <c r="F202" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A203" t="s">
-        <v>208</v>
-      </c>
-      <c r="B203">
-        <v>1</v>
-      </c>
-      <c r="C203">
-        <v>5</v>
-      </c>
-      <c r="D203">
-        <v>1</v>
-      </c>
-      <c r="E203">
-        <v>5</v>
-      </c>
-      <c r="F203" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A204" t="s">
-        <v>209</v>
-      </c>
-      <c r="B204">
-        <v>1</v>
-      </c>
-      <c r="C204">
-        <v>1</v>
-      </c>
-      <c r="D204">
-        <v>7</v>
-      </c>
-      <c r="E204">
-        <v>7</v>
-      </c>
-      <c r="F204" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A205" t="s">
-        <v>210</v>
-      </c>
-      <c r="B205">
-        <v>3</v>
-      </c>
-      <c r="C205">
-        <v>8</v>
-      </c>
-      <c r="D205">
-        <v>2</v>
-      </c>
-      <c r="E205">
-        <v>48</v>
-      </c>
-      <c r="F205" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
-        <v>211</v>
-      </c>
-      <c r="B206">
-        <v>4</v>
-      </c>
-      <c r="C206">
-        <v>5</v>
-      </c>
-      <c r="D206">
-        <v>1</v>
-      </c>
-      <c r="E206">
-        <v>20</v>
-      </c>
-      <c r="F206" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A207" t="s">
-        <v>212</v>
-      </c>
-      <c r="B207">
-        <v>6</v>
-      </c>
-      <c r="C207">
-        <v>4</v>
-      </c>
-      <c r="D207">
-        <v>6</v>
-      </c>
-      <c r="E207">
-        <v>144</v>
-      </c>
-      <c r="F207" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A208" t="s">
-        <v>213</v>
-      </c>
-      <c r="B208">
-        <v>7</v>
-      </c>
-      <c r="C208">
-        <v>8</v>
-      </c>
-      <c r="D208">
-        <v>6</v>
-      </c>
-      <c r="E208">
-        <v>336</v>
-      </c>
-      <c r="F208" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A209" t="s">
-        <v>214</v>
-      </c>
-      <c r="B209">
-        <v>5</v>
-      </c>
-      <c r="C209">
-        <v>9</v>
-      </c>
-      <c r="D209">
-        <v>5</v>
-      </c>
-      <c r="E209">
-        <v>225</v>
-      </c>
-      <c r="F209" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A210" t="s">
-        <v>215</v>
-      </c>
-      <c r="B210">
-        <v>2</v>
-      </c>
-      <c r="C210">
-        <v>9</v>
-      </c>
-      <c r="D210">
-        <v>5</v>
-      </c>
-      <c r="E210">
-        <v>90</v>
-      </c>
-      <c r="F210" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A211" t="s">
-        <v>216</v>
-      </c>
-      <c r="B211">
-        <v>4</v>
-      </c>
-      <c r="C211">
-        <v>8</v>
-      </c>
-      <c r="D211">
-        <v>5</v>
-      </c>
-      <c r="E211">
-        <v>160</v>
-      </c>
-      <c r="F211" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A212" t="s">
-        <v>217</v>
-      </c>
-      <c r="B212">
-        <v>2</v>
-      </c>
-      <c r="C212">
-        <v>8</v>
-      </c>
-      <c r="D212">
-        <v>8</v>
-      </c>
-      <c r="E212">
-        <v>128</v>
-      </c>
-      <c r="F212" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A213" t="s">
-        <v>218</v>
-      </c>
-      <c r="B213">
-        <v>5</v>
-      </c>
-      <c r="C213">
-        <v>9</v>
-      </c>
-      <c r="D213">
-        <v>4</v>
-      </c>
-      <c r="E213">
-        <v>180</v>
-      </c>
-      <c r="F213" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A214" t="s">
-        <v>219</v>
-      </c>
-      <c r="B214">
-        <v>10</v>
-      </c>
-      <c r="C214">
-        <v>2</v>
-      </c>
-      <c r="D214">
-        <v>2</v>
-      </c>
-      <c r="E214">
-        <v>40</v>
-      </c>
-      <c r="F214" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A215" t="s">
-        <v>220</v>
-      </c>
-      <c r="B215">
-        <v>10</v>
-      </c>
-      <c r="C215">
-        <v>10</v>
-      </c>
-      <c r="D215">
-        <v>3</v>
-      </c>
-      <c r="E215">
-        <v>300</v>
-      </c>
-      <c r="F215" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A216" t="s">
-        <v>221</v>
-      </c>
-      <c r="B216">
-        <v>7</v>
-      </c>
-      <c r="C216">
-        <v>4</v>
-      </c>
-      <c r="D216">
-        <v>6</v>
-      </c>
-      <c r="E216">
-        <v>168</v>
-      </c>
-      <c r="F216" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A217" t="s">
-        <v>222</v>
-      </c>
-      <c r="B217">
-        <v>7</v>
-      </c>
-      <c r="C217">
-        <v>9</v>
-      </c>
-      <c r="D217">
-        <v>1</v>
-      </c>
-      <c r="E217">
-        <v>63</v>
-      </c>
-      <c r="F217" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A218" t="s">
-        <v>223</v>
-      </c>
-      <c r="B218">
-        <v>9</v>
-      </c>
-      <c r="C218">
-        <v>9</v>
-      </c>
-      <c r="D218">
-        <v>4</v>
-      </c>
-      <c r="E218">
-        <v>324</v>
-      </c>
-      <c r="F218" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A219" t="s">
-        <v>224</v>
-      </c>
-      <c r="B219">
-        <v>9</v>
-      </c>
-      <c r="C219">
-        <v>10</v>
-      </c>
-      <c r="D219">
-        <v>9</v>
-      </c>
-      <c r="E219">
-        <v>810</v>
-      </c>
-      <c r="F219" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A220" t="s">
-        <v>225</v>
-      </c>
-      <c r="B220">
-        <v>3</v>
-      </c>
-      <c r="C220">
-        <v>7</v>
-      </c>
-      <c r="D220">
-        <v>9</v>
-      </c>
-      <c r="E220">
-        <v>189</v>
-      </c>
-      <c r="F220" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A221" t="s">
-        <v>226</v>
-      </c>
-      <c r="B221">
-        <v>9</v>
-      </c>
-      <c r="C221">
-        <v>4</v>
-      </c>
-      <c r="D221">
-        <v>3</v>
-      </c>
-      <c r="E221">
-        <v>108</v>
-      </c>
-      <c r="F221" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A222" t="s">
-        <v>227</v>
-      </c>
-      <c r="B222">
-        <v>10</v>
-      </c>
-      <c r="C222">
-        <v>3</v>
-      </c>
-      <c r="D222">
-        <v>8</v>
-      </c>
-      <c r="E222">
-        <v>240</v>
-      </c>
-      <c r="F222" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A223" t="s">
-        <v>228</v>
-      </c>
-      <c r="B223">
-        <v>4</v>
-      </c>
-      <c r="C223">
-        <v>7</v>
-      </c>
-      <c r="D223">
-        <v>2</v>
-      </c>
-      <c r="E223">
-        <v>56</v>
-      </c>
-      <c r="F223" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A224" t="s">
-        <v>229</v>
-      </c>
-      <c r="B224">
-        <v>9</v>
-      </c>
-      <c r="C224">
-        <v>4</v>
-      </c>
-      <c r="D224">
-        <v>1</v>
-      </c>
-      <c r="E224">
-        <v>36</v>
-      </c>
-      <c r="F224" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A225" t="s">
-        <v>230</v>
-      </c>
-      <c r="B225">
-        <v>2</v>
-      </c>
-      <c r="C225">
-        <v>3</v>
-      </c>
-      <c r="D225">
-        <v>2</v>
-      </c>
-      <c r="E225">
-        <v>12</v>
-      </c>
-      <c r="F225" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A226" t="s">
-        <v>231</v>
-      </c>
-      <c r="B226">
-        <v>6</v>
-      </c>
-      <c r="C226">
-        <v>4</v>
-      </c>
-      <c r="D226">
-        <v>6</v>
-      </c>
-      <c r="E226">
-        <v>144</v>
-      </c>
-      <c r="F226" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A227" t="s">
-        <v>232</v>
-      </c>
-      <c r="B227">
-        <v>6</v>
-      </c>
-      <c r="C227">
-        <v>7</v>
-      </c>
-      <c r="D227">
-        <v>4</v>
-      </c>
-      <c r="E227">
-        <v>168</v>
-      </c>
-      <c r="F227" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A228" t="s">
-        <v>233</v>
-      </c>
-      <c r="B228">
-        <v>5</v>
-      </c>
-      <c r="C228">
-        <v>7</v>
-      </c>
-      <c r="D228">
-        <v>2</v>
-      </c>
-      <c r="E228">
-        <v>70</v>
-      </c>
-      <c r="F228" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A229" t="s">
-        <v>234</v>
-      </c>
-      <c r="B229">
-        <v>1</v>
-      </c>
-      <c r="C229">
-        <v>8</v>
-      </c>
-      <c r="D229">
-        <v>5</v>
-      </c>
-      <c r="E229">
-        <v>40</v>
-      </c>
-      <c r="F229" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A230" t="s">
-        <v>235</v>
-      </c>
-      <c r="B230">
-        <v>7</v>
-      </c>
-      <c r="C230">
-        <v>9</v>
-      </c>
-      <c r="D230">
-        <v>6</v>
-      </c>
-      <c r="E230">
-        <v>378</v>
-      </c>
-      <c r="F230" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A231" t="s">
-        <v>236</v>
-      </c>
-      <c r="B231">
-        <v>2</v>
-      </c>
-      <c r="C231">
-        <v>7</v>
-      </c>
-      <c r="D231">
-        <v>6</v>
-      </c>
-      <c r="E231">
-        <v>84</v>
-      </c>
-      <c r="F231" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A232" t="s">
-        <v>237</v>
-      </c>
-      <c r="B232">
-        <v>9</v>
-      </c>
-      <c r="C232">
-        <v>10</v>
-      </c>
-      <c r="D232">
-        <v>3</v>
-      </c>
-      <c r="E232">
-        <v>270</v>
-      </c>
-      <c r="F232" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A233" t="s">
-        <v>238</v>
-      </c>
-      <c r="B233">
-        <v>2</v>
-      </c>
-      <c r="C233">
-        <v>4</v>
-      </c>
-      <c r="D233">
-        <v>2</v>
-      </c>
-      <c r="E233">
-        <v>16</v>
-      </c>
-      <c r="F233" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A234" t="s">
-        <v>239</v>
-      </c>
-      <c r="B234">
-        <v>3</v>
-      </c>
-      <c r="C234">
-        <v>7</v>
-      </c>
-      <c r="D234">
-        <v>2</v>
-      </c>
-      <c r="E234">
-        <v>42</v>
-      </c>
-      <c r="F234" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A235" t="s">
-        <v>240</v>
-      </c>
-      <c r="B235">
-        <v>3</v>
-      </c>
-      <c r="C235">
-        <v>4</v>
-      </c>
-      <c r="D235">
-        <v>7</v>
-      </c>
-      <c r="E235">
-        <v>84</v>
-      </c>
-      <c r="F235" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A236" t="s">
-        <v>241</v>
-      </c>
-      <c r="B236">
-        <v>10</v>
-      </c>
-      <c r="C236">
-        <v>6</v>
-      </c>
-      <c r="D236">
-        <v>3</v>
-      </c>
-      <c r="E236">
-        <v>180</v>
-      </c>
-      <c r="F236" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A237" t="s">
-        <v>242</v>
-      </c>
-      <c r="B237">
-        <v>5</v>
-      </c>
-      <c r="C237">
-        <v>5</v>
-      </c>
-      <c r="D237">
-        <v>4</v>
-      </c>
-      <c r="E237">
-        <v>100</v>
-      </c>
-      <c r="F237" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A238" t="s">
-        <v>243</v>
-      </c>
-      <c r="B238">
-        <v>5</v>
-      </c>
-      <c r="C238">
-        <v>9</v>
-      </c>
-      <c r="D238">
-        <v>10</v>
-      </c>
-      <c r="E238">
-        <v>450</v>
-      </c>
-      <c r="F238" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A239" t="s">
-        <v>244</v>
-      </c>
-      <c r="B239">
-        <v>2</v>
-      </c>
-      <c r="C239">
-        <v>9</v>
-      </c>
-      <c r="D239">
-        <v>5</v>
-      </c>
-      <c r="E239">
-        <v>90</v>
-      </c>
-      <c r="F239" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A240" t="s">
-        <v>245</v>
-      </c>
-      <c r="B240">
-        <v>5</v>
-      </c>
-      <c r="C240">
-        <v>1</v>
-      </c>
-      <c r="D240">
-        <v>3</v>
-      </c>
-      <c r="E240">
-        <v>15</v>
-      </c>
-      <c r="F240" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A241" t="s">
-        <v>246</v>
-      </c>
-      <c r="B241">
-        <v>5</v>
-      </c>
-      <c r="C241">
-        <v>8</v>
-      </c>
-      <c r="D241">
-        <v>1</v>
-      </c>
-      <c r="E241">
-        <v>40</v>
-      </c>
-      <c r="F241" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A242" t="s">
-        <v>247</v>
-      </c>
-      <c r="B242">
-        <v>4</v>
-      </c>
-      <c r="C242">
-        <v>4</v>
-      </c>
-      <c r="D242">
-        <v>5</v>
-      </c>
-      <c r="E242">
-        <v>80</v>
-      </c>
-      <c r="F242" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A243" t="s">
-        <v>248</v>
-      </c>
-      <c r="B243">
-        <v>6</v>
-      </c>
-      <c r="C243">
-        <v>6</v>
-      </c>
-      <c r="D243">
-        <v>5</v>
-      </c>
-      <c r="E243">
-        <v>180</v>
-      </c>
-      <c r="F243" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A244" t="s">
-        <v>249</v>
-      </c>
-      <c r="B244">
-        <v>9</v>
-      </c>
-      <c r="C244">
-        <v>9</v>
-      </c>
-      <c r="D244">
-        <v>10</v>
-      </c>
-      <c r="E244">
-        <v>810</v>
-      </c>
-      <c r="F244" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A245" t="s">
-        <v>250</v>
-      </c>
-      <c r="B245">
-        <v>5</v>
-      </c>
-      <c r="C245">
-        <v>1</v>
-      </c>
-      <c r="D245">
-        <v>2</v>
-      </c>
-      <c r="E245">
-        <v>10</v>
-      </c>
-      <c r="F245" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A246" t="s">
-        <v>251</v>
-      </c>
-      <c r="B246">
-        <v>8</v>
-      </c>
-      <c r="C246">
-        <v>9</v>
-      </c>
-      <c r="D246">
-        <v>4</v>
-      </c>
-      <c r="E246">
-        <v>288</v>
-      </c>
-      <c r="F246" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A247" t="s">
-        <v>252</v>
-      </c>
-      <c r="B247">
-        <v>6</v>
-      </c>
-      <c r="C247">
-        <v>2</v>
-      </c>
-      <c r="D247">
-        <v>2</v>
-      </c>
-      <c r="E247">
-        <v>24</v>
-      </c>
-      <c r="F247" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A248" t="s">
-        <v>253</v>
-      </c>
-      <c r="B248">
-        <v>2</v>
-      </c>
-      <c r="C248">
-        <v>3</v>
-      </c>
-      <c r="D248">
-        <v>2</v>
-      </c>
-      <c r="E248">
-        <v>12</v>
-      </c>
-      <c r="F248" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A249" t="s">
-        <v>254</v>
-      </c>
-      <c r="B249">
-        <v>2</v>
-      </c>
-      <c r="C249">
-        <v>3</v>
-      </c>
-      <c r="D249">
-        <v>9</v>
-      </c>
-      <c r="E249">
-        <v>54</v>
-      </c>
-      <c r="F249" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A250" t="s">
-        <v>255</v>
-      </c>
-      <c r="B250">
-        <v>9</v>
-      </c>
-      <c r="C250">
-        <v>3</v>
-      </c>
-      <c r="D250">
-        <v>3</v>
-      </c>
-      <c r="E250">
-        <v>81</v>
-      </c>
-      <c r="F250" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A251" t="s">
-        <v>314</v>
-      </c>
-      <c r="B251">
-        <v>7</v>
-      </c>
-      <c r="C251">
-        <v>5</v>
-      </c>
-      <c r="D251">
-        <v>1</v>
-      </c>
-      <c r="E251">
-        <v>35</v>
-      </c>
-      <c r="F251" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A252" t="s">
-        <v>256</v>
-      </c>
-      <c r="B252">
-        <v>8</v>
-      </c>
-      <c r="C252">
-        <v>9</v>
-      </c>
-      <c r="D252">
-        <v>1</v>
-      </c>
-      <c r="E252">
-        <v>72</v>
-      </c>
-      <c r="F252" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A253" t="s">
-        <v>257</v>
-      </c>
-      <c r="B253">
-        <v>4</v>
-      </c>
-      <c r="C253">
-        <v>1</v>
-      </c>
-      <c r="D253">
-        <v>5</v>
-      </c>
-      <c r="E253">
-        <v>20</v>
-      </c>
-      <c r="F253" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A254" t="s">
-        <v>258</v>
-      </c>
-      <c r="B254">
-        <v>8</v>
-      </c>
-      <c r="C254">
-        <v>10</v>
-      </c>
-      <c r="D254">
-        <v>3</v>
-      </c>
-      <c r="E254">
-        <v>240</v>
-      </c>
-      <c r="F254" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A255" t="s">
-        <v>259</v>
-      </c>
-      <c r="B255">
-        <v>10</v>
-      </c>
-      <c r="C255">
-        <v>6</v>
-      </c>
-      <c r="D255">
-        <v>4</v>
-      </c>
-      <c r="E255">
-        <v>240</v>
-      </c>
-      <c r="F255" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A256" t="s">
-        <v>260</v>
-      </c>
-      <c r="B256">
-        <v>2</v>
-      </c>
-      <c r="C256">
-        <v>1</v>
-      </c>
-      <c r="D256">
-        <v>8</v>
-      </c>
-      <c r="E256">
-        <v>16</v>
-      </c>
-      <c r="F256" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A257" t="s">
-        <v>261</v>
-      </c>
-      <c r="B257">
-        <v>3</v>
-      </c>
-      <c r="C257">
-        <v>5</v>
-      </c>
-      <c r="D257">
-        <v>10</v>
-      </c>
-      <c r="E257">
-        <v>150</v>
-      </c>
-      <c r="F257" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A258" t="s">
-        <v>262</v>
-      </c>
-      <c r="B258">
-        <v>3</v>
-      </c>
-      <c r="C258">
-        <v>6</v>
-      </c>
-      <c r="D258">
-        <v>2</v>
-      </c>
-      <c r="E258">
-        <v>36</v>
-      </c>
-      <c r="F258" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A259" t="s">
-        <v>263</v>
-      </c>
-      <c r="B259">
-        <v>3</v>
-      </c>
-      <c r="C259">
-        <v>6</v>
-      </c>
-      <c r="D259">
-        <v>10</v>
-      </c>
-      <c r="E259">
-        <v>180</v>
-      </c>
-      <c r="F259" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A260" t="s">
-        <v>264</v>
-      </c>
-      <c r="B260">
-        <v>4</v>
-      </c>
-      <c r="C260">
-        <v>10</v>
-      </c>
-      <c r="D260">
-        <v>9</v>
-      </c>
-      <c r="E260">
-        <v>360</v>
-      </c>
-      <c r="F260" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A261" t="s">
-        <v>265</v>
-      </c>
-      <c r="B261">
-        <v>3</v>
-      </c>
-      <c r="C261">
-        <v>2</v>
-      </c>
-      <c r="D261">
-        <v>7</v>
-      </c>
-      <c r="E261">
-        <v>42</v>
-      </c>
-      <c r="F261" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A262" t="s">
-        <v>34</v>
-      </c>
-      <c r="B262">
-        <v>5</v>
-      </c>
-      <c r="C262">
-        <v>4</v>
-      </c>
-      <c r="D262">
-        <v>7</v>
-      </c>
-      <c r="E262">
-        <v>140</v>
-      </c>
-      <c r="F262" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A263" t="s">
-        <v>266</v>
-      </c>
-      <c r="B263">
-        <v>1</v>
-      </c>
-      <c r="C263">
-        <v>2</v>
-      </c>
-      <c r="D263">
-        <v>3</v>
-      </c>
-      <c r="E263">
-        <v>6</v>
-      </c>
-      <c r="F263" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A264" t="s">
-        <v>315</v>
-      </c>
-      <c r="B264">
-        <v>9</v>
-      </c>
-      <c r="C264">
-        <v>7</v>
-      </c>
-      <c r="D264">
-        <v>5</v>
-      </c>
-      <c r="E264">
-        <v>315</v>
-      </c>
-      <c r="F264" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A265" t="s">
-        <v>267</v>
-      </c>
-      <c r="B265">
-        <v>1</v>
-      </c>
-      <c r="C265">
-        <v>5</v>
-      </c>
-      <c r="D265">
-        <v>6</v>
-      </c>
-      <c r="E265">
-        <v>30</v>
-      </c>
-      <c r="F265" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A266" t="s">
-        <v>268</v>
-      </c>
-      <c r="B266">
-        <v>4</v>
-      </c>
-      <c r="C266">
-        <v>10</v>
-      </c>
-      <c r="D266">
-        <v>2</v>
-      </c>
-      <c r="E266">
-        <v>80</v>
-      </c>
-      <c r="F266" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A267" t="s">
-        <v>269</v>
-      </c>
-      <c r="B267">
-        <v>6</v>
-      </c>
-      <c r="C267">
-        <v>8</v>
-      </c>
-      <c r="D267">
-        <v>8</v>
-      </c>
-      <c r="E267">
-        <v>384</v>
-      </c>
-      <c r="F267" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A268" t="s">
-        <v>270</v>
-      </c>
-      <c r="B268">
-        <v>9</v>
-      </c>
-      <c r="C268">
-        <v>7</v>
-      </c>
-      <c r="D268">
-        <v>1</v>
-      </c>
-      <c r="E268">
-        <v>63</v>
-      </c>
-      <c r="F268" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A269" t="s">
-        <v>316</v>
-      </c>
-      <c r="B269">
-        <v>10</v>
-      </c>
-      <c r="C269">
-        <v>7</v>
-      </c>
-      <c r="D269">
-        <v>9</v>
-      </c>
-      <c r="E269">
-        <v>630</v>
-      </c>
-      <c r="F269" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A270" t="s">
-        <v>271</v>
-      </c>
-      <c r="B270">
-        <v>1</v>
-      </c>
-      <c r="C270">
-        <v>8</v>
-      </c>
-      <c r="D270">
-        <v>2</v>
-      </c>
-      <c r="E270">
-        <v>16</v>
-      </c>
-      <c r="F270" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A271" t="s">
-        <v>272</v>
-      </c>
-      <c r="B271">
-        <v>6</v>
-      </c>
-      <c r="C271">
-        <v>3</v>
-      </c>
-      <c r="D271">
-        <v>8</v>
-      </c>
-      <c r="E271">
-        <v>144</v>
-      </c>
-      <c r="F271" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A272" t="s">
-        <v>273</v>
-      </c>
-      <c r="B272" s="4">
-        <v>10</v>
-      </c>
-      <c r="C272">
-        <v>6</v>
-      </c>
-      <c r="D272">
-        <v>3</v>
-      </c>
-      <c r="E272">
-        <v>180</v>
-      </c>
-      <c r="F272" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A273" t="s">
-        <v>274</v>
-      </c>
-      <c r="B273">
-        <v>1</v>
-      </c>
-      <c r="C273">
-        <v>9</v>
-      </c>
-      <c r="D273">
-        <v>9</v>
-      </c>
-      <c r="E273">
-        <v>81</v>
-      </c>
-      <c r="F273" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A274" t="s">
-        <v>317</v>
-      </c>
-      <c r="B274">
-        <v>1</v>
-      </c>
-      <c r="C274">
-        <v>5</v>
-      </c>
-      <c r="D274">
-        <v>10</v>
-      </c>
-      <c r="E274">
-        <v>50</v>
-      </c>
-      <c r="F274" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A275" t="s">
-        <v>275</v>
-      </c>
-      <c r="B275">
-        <v>9</v>
-      </c>
-      <c r="C275">
-        <v>8</v>
-      </c>
-      <c r="D275">
-        <v>4</v>
-      </c>
-      <c r="E275">
-        <v>288</v>
-      </c>
-      <c r="F275" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A276" t="s">
-        <v>276</v>
-      </c>
-      <c r="B276">
-        <v>6</v>
-      </c>
-      <c r="C276">
-        <v>9</v>
-      </c>
-      <c r="D276">
-        <v>6</v>
-      </c>
-      <c r="E276">
-        <v>324</v>
-      </c>
-      <c r="F276" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A277" t="s">
-        <v>277</v>
-      </c>
-      <c r="B277">
-        <v>8</v>
-      </c>
-      <c r="C277">
-        <v>8</v>
-      </c>
-      <c r="D277">
-        <v>8</v>
-      </c>
-      <c r="E277">
-        <v>512</v>
-      </c>
-      <c r="F277" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A278" t="s">
-        <v>278</v>
-      </c>
-      <c r="B278">
-        <v>3</v>
-      </c>
-      <c r="C278">
-        <v>8</v>
-      </c>
-      <c r="D278">
-        <v>2</v>
-      </c>
-      <c r="E278">
-        <v>48</v>
-      </c>
-      <c r="F278" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A279" t="s">
-        <v>279</v>
-      </c>
-      <c r="B279">
-        <v>9</v>
-      </c>
-      <c r="C279">
-        <v>3</v>
-      </c>
-      <c r="D279">
-        <v>4</v>
-      </c>
-      <c r="E279">
-        <v>108</v>
-      </c>
-      <c r="F279" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A280" t="s">
-        <v>318</v>
-      </c>
-      <c r="B280">
-        <v>4</v>
-      </c>
-      <c r="C280">
-        <v>9</v>
-      </c>
-      <c r="D280">
-        <v>7</v>
-      </c>
-      <c r="E280">
-        <v>252</v>
-      </c>
-      <c r="F280" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A281" t="s">
-        <v>280</v>
-      </c>
-      <c r="B281">
-        <v>5</v>
-      </c>
-      <c r="C281">
-        <v>10</v>
-      </c>
-      <c r="D281">
-        <v>2</v>
-      </c>
-      <c r="E281">
-        <v>100</v>
-      </c>
-      <c r="F281" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A282" t="s">
-        <v>281</v>
-      </c>
-      <c r="B282">
-        <v>1</v>
-      </c>
-      <c r="C282">
-        <v>1</v>
-      </c>
-      <c r="D282">
-        <v>8</v>
-      </c>
-      <c r="E282">
-        <v>8</v>
-      </c>
-      <c r="F282" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A283" t="s">
-        <v>282</v>
-      </c>
-      <c r="B283">
-        <v>2</v>
-      </c>
-      <c r="C283">
-        <v>6</v>
-      </c>
-      <c r="D283">
-        <v>1</v>
-      </c>
-      <c r="E283">
-        <v>12</v>
-      </c>
-      <c r="F283" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A284" t="s">
-        <v>283</v>
-      </c>
-      <c r="B284">
-        <v>7</v>
-      </c>
-      <c r="C284">
-        <v>4</v>
-      </c>
-      <c r="D284">
-        <v>10</v>
-      </c>
-      <c r="E284">
-        <v>280</v>
-      </c>
-      <c r="F284" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A285" t="s">
-        <v>285</v>
-      </c>
-      <c r="B285">
-        <v>10</v>
-      </c>
-      <c r="C285">
-        <v>10</v>
-      </c>
-      <c r="D285">
-        <v>5</v>
-      </c>
-      <c r="E285">
-        <v>500</v>
-      </c>
-      <c r="F285" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A286" t="s">
-        <v>286</v>
-      </c>
-      <c r="B286">
-        <v>4</v>
-      </c>
-      <c r="C286">
-        <v>4</v>
-      </c>
-      <c r="D286">
-        <v>2</v>
-      </c>
-      <c r="E286">
-        <v>32</v>
-      </c>
-      <c r="F286" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A287" t="s">
-        <v>135</v>
-      </c>
-      <c r="B287">
-        <v>7</v>
-      </c>
-      <c r="C287">
-        <v>4</v>
-      </c>
-      <c r="D287">
-        <v>1</v>
-      </c>
-      <c r="E287">
-        <v>28</v>
-      </c>
-      <c r="F287" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A288" t="s">
-        <v>287</v>
-      </c>
-      <c r="B288">
-        <v>8</v>
-      </c>
-      <c r="C288">
-        <v>7</v>
-      </c>
-      <c r="D288">
-        <v>4</v>
-      </c>
-      <c r="E288">
-        <v>224</v>
-      </c>
-      <c r="F288" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A289" t="s">
-        <v>288</v>
-      </c>
-      <c r="B289">
-        <v>3</v>
-      </c>
-      <c r="C289">
-        <v>1</v>
-      </c>
-      <c r="D289">
-        <v>9</v>
-      </c>
-      <c r="E289">
-        <v>27</v>
-      </c>
-      <c r="F289" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A290" t="s">
-        <v>289</v>
-      </c>
-      <c r="B290">
-        <v>3</v>
-      </c>
-      <c r="C290">
-        <v>7</v>
-      </c>
-      <c r="D290">
-        <v>3</v>
-      </c>
-      <c r="E290">
-        <v>63</v>
-      </c>
-      <c r="F290" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A291" t="s">
-        <v>319</v>
-      </c>
-      <c r="B291">
-        <v>7</v>
-      </c>
-      <c r="C291">
-        <v>4</v>
-      </c>
-      <c r="D291">
-        <v>4</v>
-      </c>
-      <c r="E291">
-        <v>112</v>
-      </c>
-      <c r="F291" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A292" t="s">
-        <v>290</v>
-      </c>
-      <c r="B292">
-        <v>10</v>
-      </c>
-      <c r="C292">
-        <v>6</v>
-      </c>
-      <c r="D292">
-        <v>7</v>
-      </c>
-      <c r="E292">
-        <v>420</v>
-      </c>
-      <c r="F292" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A293" t="s">
-        <v>21</v>
-      </c>
-      <c r="B293">
-        <v>4</v>
-      </c>
-      <c r="C293">
-        <v>8</v>
-      </c>
-      <c r="D293">
-        <v>3</v>
-      </c>
-      <c r="E293">
-        <v>96</v>
-      </c>
-      <c r="F293" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A294" t="s">
-        <v>291</v>
-      </c>
-      <c r="B294">
-        <v>5</v>
-      </c>
-      <c r="C294">
-        <v>9</v>
-      </c>
-      <c r="D294">
-        <v>3</v>
-      </c>
-      <c r="E294">
-        <v>135</v>
-      </c>
-      <c r="F294" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A295" t="s">
-        <v>292</v>
-      </c>
-      <c r="B295">
-        <v>1</v>
-      </c>
-      <c r="C295">
-        <v>6</v>
-      </c>
-      <c r="D295">
-        <v>9</v>
-      </c>
-      <c r="E295">
-        <v>54</v>
-      </c>
-      <c r="F295" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A296" t="s">
-        <v>294</v>
-      </c>
-      <c r="B296">
-        <v>4</v>
-      </c>
-      <c r="C296">
-        <v>8</v>
-      </c>
-      <c r="D296">
-        <v>5</v>
-      </c>
-      <c r="E296">
-        <v>160</v>
-      </c>
-      <c r="F296" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A297" t="s">
-        <v>320</v>
-      </c>
-      <c r="B297">
-        <v>3</v>
-      </c>
-      <c r="C297">
-        <v>8</v>
-      </c>
-      <c r="D297">
-        <v>4</v>
-      </c>
-      <c r="E297">
-        <v>96</v>
-      </c>
-      <c r="F297" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A298" t="s">
-        <v>295</v>
-      </c>
-      <c r="B298">
-        <v>4</v>
-      </c>
-      <c r="C298">
-        <v>6</v>
-      </c>
-      <c r="D298">
-        <v>10</v>
-      </c>
-      <c r="E298">
-        <v>240</v>
-      </c>
-      <c r="F298" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A299" t="s">
-        <v>229</v>
-      </c>
-      <c r="B299">
-        <v>9</v>
-      </c>
-      <c r="C299">
-        <v>6</v>
-      </c>
-      <c r="D299">
-        <v>5</v>
-      </c>
-      <c r="E299">
-        <v>270</v>
-      </c>
-      <c r="F299" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A300" t="s">
-        <v>296</v>
-      </c>
-      <c r="B300">
-        <v>9</v>
-      </c>
-      <c r="C300">
-        <v>5</v>
-      </c>
-      <c r="D300">
-        <v>5</v>
-      </c>
-      <c r="E300">
-        <v>225</v>
-      </c>
-      <c r="F300" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A301" t="s">
-        <v>297</v>
-      </c>
-      <c r="B301">
-        <v>4</v>
-      </c>
-      <c r="C301">
-        <v>5</v>
-      </c>
-      <c r="D301">
-        <v>2</v>
-      </c>
-      <c r="E301">
-        <v>40</v>
-      </c>
-      <c r="F301" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A302" t="s">
-        <v>298</v>
-      </c>
-      <c r="B302">
-        <v>3</v>
-      </c>
-      <c r="C302">
-        <v>9</v>
-      </c>
-      <c r="D302">
-        <v>1</v>
-      </c>
-      <c r="E302">
-        <v>27</v>
-      </c>
-      <c r="F302" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A303" t="s">
-        <v>299</v>
-      </c>
-      <c r="B303">
-        <v>2</v>
-      </c>
-      <c r="C303">
-        <v>7</v>
-      </c>
-      <c r="D303">
-        <v>9</v>
-      </c>
-      <c r="E303">
-        <v>126</v>
-      </c>
-      <c r="F303" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A304" t="s">
-        <v>300</v>
-      </c>
-      <c r="B304">
-        <v>10</v>
-      </c>
-      <c r="C304">
-        <v>2</v>
-      </c>
-      <c r="D304">
-        <v>7</v>
-      </c>
-      <c r="E304">
-        <v>140</v>
-      </c>
-      <c r="F304" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A305" t="s">
-        <v>301</v>
-      </c>
-      <c r="B305">
-        <v>4</v>
-      </c>
-      <c r="C305">
-        <v>6</v>
-      </c>
-      <c r="D305">
-        <v>4</v>
-      </c>
-      <c r="E305">
-        <v>96</v>
-      </c>
-      <c r="F305" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A306" t="s">
-        <v>302</v>
-      </c>
-      <c r="B306">
-        <v>10</v>
-      </c>
-      <c r="C306">
-        <v>1</v>
-      </c>
-      <c r="D306">
-        <v>7</v>
-      </c>
-      <c r="E306">
-        <v>70</v>
-      </c>
-      <c r="F306" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A307" t="s">
-        <v>303</v>
-      </c>
-      <c r="B307">
-        <v>3</v>
-      </c>
-      <c r="C307">
-        <v>6</v>
-      </c>
-      <c r="D307">
-        <v>4</v>
-      </c>
-      <c r="E307">
-        <v>72</v>
-      </c>
-      <c r="F307" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A308" t="s">
-        <v>305</v>
-      </c>
-      <c r="B308">
-        <v>5</v>
-      </c>
-      <c r="C308">
-        <v>8</v>
-      </c>
-      <c r="D308">
-        <v>2</v>
-      </c>
-      <c r="E308">
-        <v>80</v>
-      </c>
-      <c r="F308" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A309" t="s">
-        <v>306</v>
-      </c>
-      <c r="B309">
-        <v>9</v>
-      </c>
-      <c r="C309">
-        <v>8</v>
-      </c>
-      <c r="D309">
-        <v>1</v>
-      </c>
-      <c r="E309">
-        <v>72</v>
-      </c>
-      <c r="F309" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A310" t="s">
-        <v>307</v>
-      </c>
-      <c r="B310" s="4">
-        <v>6</v>
-      </c>
-      <c r="C310">
-        <v>9</v>
-      </c>
-      <c r="D310">
-        <v>5</v>
-      </c>
-      <c r="E310">
-        <v>270</v>
-      </c>
-      <c r="F310" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A311" t="s">
-        <v>308</v>
-      </c>
-      <c r="B311" s="4">
-        <v>9</v>
-      </c>
-      <c r="C311">
-        <v>9</v>
-      </c>
-      <c r="D311">
-        <v>7</v>
-      </c>
-      <c r="E311">
-        <v>567</v>
-      </c>
-      <c r="F311" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A312" t="s">
-        <v>309</v>
-      </c>
-      <c r="B312" s="4">
-        <v>6</v>
-      </c>
-      <c r="C312">
-        <v>7</v>
-      </c>
-      <c r="D312">
-        <v>9</v>
-      </c>
-      <c r="E312">
-        <v>378</v>
-      </c>
-      <c r="F312" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A313" t="s">
-        <v>310</v>
-      </c>
-      <c r="B313" s="4">
-        <v>1</v>
-      </c>
-      <c r="C313">
-        <v>6</v>
-      </c>
-      <c r="D313">
-        <v>5</v>
-      </c>
-      <c r="E313">
-        <v>30</v>
-      </c>
-      <c r="F313" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A314" t="s">
-        <v>119</v>
-      </c>
-      <c r="B314" s="4">
-        <v>8</v>
-      </c>
-      <c r="C314">
-        <v>1</v>
-      </c>
-      <c r="D314">
-        <v>3</v>
-      </c>
-      <c r="E314">
-        <v>24</v>
-      </c>
-      <c r="F314" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A315" t="s">
-        <v>311</v>
-      </c>
-      <c r="B315">
-        <v>8</v>
-      </c>
-      <c r="C315">
-        <v>1</v>
-      </c>
-      <c r="D315">
-        <v>3</v>
-      </c>
-      <c r="E315">
-        <v>24</v>
-      </c>
-      <c r="F315" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A316" t="s">
-        <v>284</v>
-      </c>
-      <c r="B316">
-        <v>9</v>
-      </c>
-      <c r="C316">
-        <v>6</v>
-      </c>
-      <c r="D316">
-        <v>7</v>
-      </c>
-      <c r="E316">
-        <v>378</v>
-      </c>
-      <c r="F316" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A317" t="s">
-        <v>293</v>
-      </c>
-      <c r="B317">
-        <v>8</v>
-      </c>
-      <c r="C317">
-        <v>3</v>
-      </c>
-      <c r="D317">
-        <v>2</v>
-      </c>
-      <c r="E317">
-        <v>48</v>
-      </c>
-      <c r="F317" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A318" t="s">
-        <v>304</v>
-      </c>
-      <c r="B318">
-        <v>1</v>
-      </c>
-      <c r="C318">
-        <v>3</v>
-      </c>
-      <c r="D318">
-        <v>5</v>
-      </c>
-      <c r="E318">
-        <v>15</v>
-      </c>
-      <c r="F318" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>